<commit_message>
update figure for custom dataset
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17025" windowHeight="9075" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -182,10 +182,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"input type": &lt;"image_data", "table_data" or "time_series"&gt;,</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;key name&gt;: &lt;value&gt;,</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -194,10 +190,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"input type": "image_data",</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>"name": "file",</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -226,10 +218,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"input type": "table_data",</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>"name": "MedInc",</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -283,6 +271,70 @@
   </si>
   <si>
     <t>"target": 3.58500,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"is_analysis": &lt;"True" or "False"&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>is_analysis:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies whether the dataset analyzed in the AI Dashboard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>task:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the machine learning task</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>input_type:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"input_type": &lt;"image_data", "table_data" or "time_series"&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"input_type": "image_data",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"input_type": "table_data",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the data type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>keys:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the keys described in info.json for train, validation and test dataset</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>id:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the sample number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>target:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the target value</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1957,13 +2009,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132521</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>207065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>231913</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2016,13 +2068,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>198782</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2065,13 +2117,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>165652</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>82826</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2114,13 +2166,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>207065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>231913</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2173,13 +2225,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>72</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>107676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>198782</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2222,13 +2274,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>140804</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>66261</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2271,13 +2323,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>78</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>198782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>223631</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2330,13 +2382,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>124240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>182217</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>91109</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2382,13 +2434,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>91109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>124239</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2434,13 +2486,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>215348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2493,13 +2545,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>165652</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2545,13 +2597,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>107673</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2931,10 +2983,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AQ89"/>
+  <dimension ref="B2:AQ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AN43" sqref="AN43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3770,7 +3822,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -3816,7 +3868,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -3862,7 +3914,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -3889,7 +3941,7 @@
       <c r="AC38" s="10"/>
       <c r="AD38" s="10"/>
       <c r="AE38" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AF38" s="10"/>
       <c r="AG38" s="10"/>
@@ -3907,10 +3959,10 @@
     <row r="39" spans="2:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C39" s="9"/>
       <c r="D39" s="10"/>
-      <c r="E39" s="10"/>
-      <c r="F39" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="E39" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -3954,10 +4006,10 @@
       <c r="C40" s="9"/>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="F40" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="10"/>
       <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
@@ -4001,10 +4053,10 @@
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="G41" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
@@ -4049,7 +4101,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
@@ -4093,10 +4145,10 @@
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -4119,7 +4171,7 @@
       <c r="AC43" s="10"/>
       <c r="AD43" s="10"/>
       <c r="AE43" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AF43" s="10"/>
       <c r="AG43" s="10"/>
@@ -4140,7 +4192,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
@@ -4185,10 +4237,10 @@
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="G45" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
@@ -4233,7 +4285,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
@@ -4277,10 +4329,10 @@
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
-      <c r="G47" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
@@ -4324,7 +4376,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
@@ -4366,10 +4418,10 @@
       <c r="C49" s="9"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
-      <c r="F49" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
@@ -4407,621 +4459,202 @@
       <c r="AQ49" s="11"/>
     </row>
     <row r="50" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C50" s="12"/>
-      <c r="D50" s="13" t="s">
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="10"/>
+      <c r="Q50" s="10"/>
+      <c r="R50" s="10"/>
+      <c r="S50" s="10"/>
+      <c r="T50" s="10"/>
+      <c r="U50" s="10"/>
+      <c r="V50" s="10"/>
+      <c r="W50" s="10"/>
+      <c r="X50" s="10"/>
+      <c r="Y50" s="10"/>
+      <c r="Z50" s="11"/>
+      <c r="AB50" s="9"/>
+      <c r="AC50" s="10"/>
+      <c r="AD50" s="10"/>
+      <c r="AE50" s="10"/>
+      <c r="AF50" s="10"/>
+      <c r="AG50" s="10"/>
+      <c r="AH50" s="10"/>
+      <c r="AI50" s="10"/>
+      <c r="AJ50" s="10"/>
+      <c r="AK50" s="10"/>
+      <c r="AL50" s="10"/>
+      <c r="AM50" s="10"/>
+      <c r="AN50" s="10"/>
+      <c r="AO50" s="10"/>
+      <c r="AP50" s="10"/>
+      <c r="AQ50" s="11"/>
+    </row>
+    <row r="51" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C51" s="12"/>
+      <c r="D51" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="13"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="13"/>
-      <c r="R50" s="13"/>
-      <c r="S50" s="13"/>
-      <c r="T50" s="13"/>
-      <c r="U50" s="13"/>
-      <c r="V50" s="13"/>
-      <c r="W50" s="13"/>
-      <c r="X50" s="13"/>
-      <c r="Y50" s="13"/>
-      <c r="Z50" s="14"/>
-      <c r="AB50" s="12"/>
-      <c r="AC50" s="13"/>
-      <c r="AD50" s="13"/>
-      <c r="AE50" s="13"/>
-      <c r="AF50" s="13"/>
-      <c r="AG50" s="13"/>
-      <c r="AH50" s="13"/>
-      <c r="AI50" s="13"/>
-      <c r="AJ50" s="13"/>
-      <c r="AK50" s="13"/>
-      <c r="AL50" s="13"/>
-      <c r="AM50" s="13"/>
-      <c r="AN50" s="13"/>
-      <c r="AO50" s="13"/>
-      <c r="AP50" s="13"/>
-      <c r="AQ50" s="14"/>
-    </row>
-    <row r="52" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C52" s="5" t="s">
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13"/>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+      <c r="V51" s="13"/>
+      <c r="W51" s="13"/>
+      <c r="X51" s="13"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="14"/>
+      <c r="AB51" s="12"/>
+      <c r="AC51" s="13"/>
+      <c r="AD51" s="13"/>
+      <c r="AE51" s="13"/>
+      <c r="AF51" s="13"/>
+      <c r="AG51" s="13"/>
+      <c r="AH51" s="13"/>
+      <c r="AI51" s="13"/>
+      <c r="AJ51" s="13"/>
+      <c r="AK51" s="13"/>
+      <c r="AL51" s="13"/>
+      <c r="AM51" s="13"/>
+      <c r="AN51" s="13"/>
+      <c r="AO51" s="13"/>
+      <c r="AP51" s="13"/>
+      <c r="AQ51" s="14"/>
+    </row>
+    <row r="53" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD53" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F54" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE54" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E55" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD55" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F56" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE56" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E57" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F58" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E59" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F60" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C63" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C53" s="6" t="s">
+    <row r="64" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C64" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-      <c r="U53" s="7"/>
-      <c r="V53" s="7"/>
-      <c r="W53" s="7"/>
-      <c r="X53" s="7"/>
-      <c r="Y53" s="7"/>
-      <c r="Z53" s="7"/>
-      <c r="AA53" s="7"/>
-      <c r="AB53" s="7" t="s">
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
+      <c r="J64" s="7"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+      <c r="Y64" s="7"/>
+      <c r="Z64" s="7"/>
+      <c r="AA64" s="7"/>
+      <c r="AB64" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AC53" s="7"/>
-      <c r="AD53" s="7"/>
-      <c r="AE53" s="7"/>
-      <c r="AF53" s="7"/>
-      <c r="AG53" s="7"/>
-      <c r="AH53" s="7"/>
-      <c r="AI53" s="7"/>
-      <c r="AJ53" s="7"/>
-      <c r="AK53" s="7"/>
-      <c r="AL53" s="7"/>
-      <c r="AM53" s="7"/>
-      <c r="AN53" s="7"/>
-      <c r="AO53" s="7"/>
-      <c r="AP53" s="7"/>
-      <c r="AQ53" s="8"/>
-    </row>
-    <row r="54" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C54" s="9"/>
-      <c r="D54" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
-      <c r="M54" s="10"/>
-      <c r="N54" s="10"/>
-      <c r="O54" s="10"/>
-      <c r="P54" s="10"/>
-      <c r="Q54" s="10"/>
-      <c r="R54" s="10"/>
-      <c r="S54" s="10"/>
-      <c r="T54" s="10"/>
-      <c r="U54" s="10"/>
-      <c r="V54" s="10"/>
-      <c r="W54" s="10"/>
-      <c r="X54" s="10"/>
-      <c r="Y54" s="10"/>
-      <c r="Z54" s="10"/>
-      <c r="AA54" s="10"/>
-      <c r="AB54" s="10"/>
-      <c r="AC54" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD54" s="10"/>
-      <c r="AE54" s="10"/>
-      <c r="AF54" s="10"/>
-      <c r="AG54" s="10"/>
-      <c r="AH54" s="10"/>
-      <c r="AI54" s="10"/>
-      <c r="AJ54" s="10"/>
-      <c r="AK54" s="10"/>
-      <c r="AL54" s="10"/>
-      <c r="AM54" s="10"/>
-      <c r="AN54" s="10"/>
-      <c r="AO54" s="10"/>
-      <c r="AP54" s="10"/>
-      <c r="AQ54" s="11"/>
-    </row>
-    <row r="55" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C55" s="9"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F55" s="10"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10"/>
-      <c r="I55" s="10"/>
-      <c r="J55" s="10"/>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="10"/>
-      <c r="Q55" s="10"/>
-      <c r="R55" s="10"/>
-      <c r="S55" s="10"/>
-      <c r="T55" s="10"/>
-      <c r="U55" s="10"/>
-      <c r="V55" s="10"/>
-      <c r="W55" s="10"/>
-      <c r="X55" s="10"/>
-      <c r="Y55" s="10"/>
-      <c r="Z55" s="10"/>
-      <c r="AA55" s="10"/>
-      <c r="AB55" s="10"/>
-      <c r="AC55" s="10"/>
-      <c r="AD55" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE55" s="10"/>
-      <c r="AF55" s="10"/>
-      <c r="AG55" s="10"/>
-      <c r="AH55" s="10"/>
-      <c r="AI55" s="10"/>
-      <c r="AJ55" s="10"/>
-      <c r="AK55" s="10"/>
-      <c r="AL55" s="10"/>
-      <c r="AM55" s="10"/>
-      <c r="AN55" s="10"/>
-      <c r="AO55" s="10"/>
-      <c r="AP55" s="10"/>
-      <c r="AQ55" s="11"/>
-    </row>
-    <row r="56" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C56" s="9"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
-      <c r="N56" s="10"/>
-      <c r="O56" s="10"/>
-      <c r="P56" s="10"/>
-      <c r="Q56" s="10"/>
-      <c r="R56" s="10"/>
-      <c r="S56" s="10"/>
-      <c r="T56" s="10"/>
-      <c r="U56" s="10"/>
-      <c r="V56" s="10"/>
-      <c r="W56" s="10"/>
-      <c r="X56" s="10"/>
-      <c r="Y56" s="10"/>
-      <c r="Z56" s="10"/>
-      <c r="AA56" s="10"/>
-      <c r="AB56" s="10"/>
-      <c r="AC56" s="10"/>
-      <c r="AD56" s="10"/>
-      <c r="AE56" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF56" s="10"/>
-      <c r="AG56" s="10"/>
-      <c r="AH56" s="10"/>
-      <c r="AI56" s="10"/>
-      <c r="AJ56" s="10"/>
-      <c r="AK56" s="10"/>
-      <c r="AL56" s="10"/>
-      <c r="AM56" s="10"/>
-      <c r="AN56" s="10"/>
-      <c r="AO56" s="10"/>
-      <c r="AP56" s="10"/>
-      <c r="AQ56" s="11"/>
-    </row>
-    <row r="57" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C57" s="9"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F57" s="10"/>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
-      <c r="M57" s="10"/>
-      <c r="N57" s="10"/>
-      <c r="O57" s="10"/>
-      <c r="P57" s="10"/>
-      <c r="Q57" s="10"/>
-      <c r="R57" s="10"/>
-      <c r="S57" s="10"/>
-      <c r="T57" s="10"/>
-      <c r="U57" s="10"/>
-      <c r="V57" s="10"/>
-      <c r="W57" s="10"/>
-      <c r="X57" s="10"/>
-      <c r="Y57" s="10"/>
-      <c r="Z57" s="10"/>
-      <c r="AA57" s="10"/>
-      <c r="AB57" s="10"/>
-      <c r="AC57" s="10"/>
-      <c r="AD57" s="10"/>
-      <c r="AE57" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF57" s="10"/>
-      <c r="AG57" s="10"/>
-      <c r="AH57" s="10"/>
-      <c r="AI57" s="10"/>
-      <c r="AJ57" s="10"/>
-      <c r="AK57" s="10"/>
-      <c r="AL57" s="10"/>
-      <c r="AM57" s="10"/>
-      <c r="AN57" s="10"/>
-      <c r="AO57" s="10"/>
-      <c r="AP57" s="10"/>
-      <c r="AQ57" s="11"/>
-    </row>
-    <row r="58" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C58" s="9"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10"/>
-      <c r="I58" s="10"/>
-      <c r="J58" s="10"/>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="10"/>
-      <c r="S58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10"/>
-      <c r="V58" s="10"/>
-      <c r="W58" s="10"/>
-      <c r="X58" s="10"/>
-      <c r="Y58" s="10"/>
-      <c r="Z58" s="10"/>
-      <c r="AA58" s="10"/>
-      <c r="AB58" s="10"/>
-      <c r="AC58" s="10"/>
-      <c r="AD58" s="10"/>
-      <c r="AE58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF58" s="10"/>
-      <c r="AG58" s="10"/>
-      <c r="AH58" s="10"/>
-      <c r="AI58" s="10"/>
-      <c r="AJ58" s="10"/>
-      <c r="AK58" s="10"/>
-      <c r="AL58" s="10"/>
-      <c r="AM58" s="10"/>
-      <c r="AN58" s="10"/>
-      <c r="AO58" s="10"/>
-      <c r="AP58" s="10"/>
-      <c r="AQ58" s="11"/>
-    </row>
-    <row r="59" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C59" s="9"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H59" s="10"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="10"/>
-      <c r="K59" s="10"/>
-      <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
-      <c r="Q59" s="10"/>
-      <c r="R59" s="10"/>
-      <c r="S59" s="10"/>
-      <c r="T59" s="10"/>
-      <c r="U59" s="10"/>
-      <c r="V59" s="10"/>
-      <c r="W59" s="10"/>
-      <c r="X59" s="10"/>
-      <c r="Y59" s="10"/>
-      <c r="Z59" s="10"/>
-      <c r="AA59" s="10"/>
-      <c r="AB59" s="10"/>
-      <c r="AC59" s="10"/>
-      <c r="AD59" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE59" s="10"/>
-      <c r="AF59" s="10"/>
-      <c r="AG59" s="10"/>
-      <c r="AH59" s="10"/>
-      <c r="AI59" s="10"/>
-      <c r="AJ59" s="10"/>
-      <c r="AK59" s="10"/>
-      <c r="AL59" s="10"/>
-      <c r="AM59" s="10"/>
-      <c r="AN59" s="10"/>
-      <c r="AO59" s="10"/>
-      <c r="AP59" s="10"/>
-      <c r="AQ59" s="11"/>
-    </row>
-    <row r="60" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C60" s="9"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I60" s="10"/>
-      <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
-      <c r="L60" s="10"/>
-      <c r="M60" s="10"/>
-      <c r="N60" s="10"/>
-      <c r="O60" s="10"/>
-      <c r="P60" s="10"/>
-      <c r="Q60" s="10"/>
-      <c r="R60" s="10"/>
-      <c r="S60" s="10"/>
-      <c r="T60" s="10"/>
-      <c r="U60" s="10"/>
-      <c r="V60" s="10"/>
-      <c r="W60" s="10"/>
-      <c r="X60" s="10"/>
-      <c r="Y60" s="10"/>
-      <c r="Z60" s="10"/>
-      <c r="AA60" s="10"/>
-      <c r="AB60" s="10"/>
-      <c r="AC60" s="10"/>
-      <c r="AD60" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE60" s="10"/>
-      <c r="AF60" s="10"/>
-      <c r="AG60" s="10"/>
-      <c r="AH60" s="10"/>
-      <c r="AI60" s="10"/>
-      <c r="AJ60" s="10"/>
-      <c r="AK60" s="10"/>
-      <c r="AL60" s="10"/>
-      <c r="AM60" s="10"/>
-      <c r="AN60" s="10"/>
-      <c r="AO60" s="10"/>
-      <c r="AP60" s="10"/>
-      <c r="AQ60" s="11"/>
-    </row>
-    <row r="61" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C61" s="9"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10"/>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
-      <c r="Q61" s="10"/>
-      <c r="R61" s="10"/>
-      <c r="S61" s="10"/>
-      <c r="T61" s="10"/>
-      <c r="U61" s="10"/>
-      <c r="V61" s="10"/>
-      <c r="W61" s="10"/>
-      <c r="X61" s="10"/>
-      <c r="Y61" s="10"/>
-      <c r="Z61" s="10"/>
-      <c r="AA61" s="10"/>
-      <c r="AB61" s="10"/>
-      <c r="AC61" s="10"/>
-      <c r="AD61" s="10"/>
-      <c r="AE61" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF61" s="10"/>
-      <c r="AG61" s="10"/>
-      <c r="AH61" s="10"/>
-      <c r="AI61" s="10"/>
-      <c r="AJ61" s="10"/>
-      <c r="AK61" s="10"/>
-      <c r="AL61" s="10"/>
-      <c r="AM61" s="10"/>
-      <c r="AN61" s="10"/>
-      <c r="AO61" s="10"/>
-      <c r="AP61" s="10"/>
-      <c r="AQ61" s="11"/>
-    </row>
-    <row r="62" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C62" s="9"/>
-      <c r="D62" s="10"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="10"/>
-      <c r="G62" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
-      <c r="O62" s="10"/>
-      <c r="P62" s="10"/>
-      <c r="Q62" s="10"/>
-      <c r="R62" s="10"/>
-      <c r="S62" s="10"/>
-      <c r="T62" s="10"/>
-      <c r="U62" s="10"/>
-      <c r="V62" s="10"/>
-      <c r="W62" s="10"/>
-      <c r="X62" s="10"/>
-      <c r="Y62" s="10"/>
-      <c r="Z62" s="10"/>
-      <c r="AA62" s="10"/>
-      <c r="AB62" s="10"/>
-      <c r="AC62" s="10"/>
-      <c r="AD62" s="10"/>
-      <c r="AE62" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF62" s="10"/>
-      <c r="AG62" s="10"/>
-      <c r="AH62" s="10"/>
-      <c r="AI62" s="10"/>
-      <c r="AJ62" s="10"/>
-      <c r="AK62" s="10"/>
-      <c r="AL62" s="10"/>
-      <c r="AM62" s="10"/>
-      <c r="AN62" s="10"/>
-      <c r="AO62" s="10"/>
-      <c r="AP62" s="10"/>
-      <c r="AQ62" s="11"/>
-    </row>
-    <row r="63" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C63" s="9"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10"/>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
-      <c r="O63" s="10"/>
-      <c r="P63" s="10"/>
-      <c r="Q63" s="10"/>
-      <c r="R63" s="10"/>
-      <c r="S63" s="10"/>
-      <c r="T63" s="10"/>
-      <c r="U63" s="10"/>
-      <c r="V63" s="10"/>
-      <c r="W63" s="10"/>
-      <c r="X63" s="10"/>
-      <c r="Y63" s="10"/>
-      <c r="Z63" s="10"/>
-      <c r="AA63" s="10"/>
-      <c r="AB63" s="10"/>
-      <c r="AC63" s="10"/>
-      <c r="AD63" s="10"/>
-      <c r="AE63" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF63" s="10"/>
-      <c r="AG63" s="10"/>
-      <c r="AH63" s="10"/>
-      <c r="AI63" s="10"/>
-      <c r="AJ63" s="10"/>
-      <c r="AK63" s="10"/>
-      <c r="AL63" s="10"/>
-      <c r="AM63" s="10"/>
-      <c r="AN63" s="10"/>
-      <c r="AO63" s="10"/>
-      <c r="AP63" s="10"/>
-      <c r="AQ63" s="11"/>
-    </row>
-    <row r="64" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C64" s="9"/>
-      <c r="D64" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" s="10"/>
-      <c r="F64" s="10"/>
-      <c r="G64" s="10"/>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
-      <c r="O64" s="10"/>
-      <c r="P64" s="10"/>
-      <c r="Q64" s="10"/>
-      <c r="R64" s="10"/>
-      <c r="S64" s="10"/>
-      <c r="T64" s="10"/>
-      <c r="U64" s="10"/>
-      <c r="V64" s="10"/>
-      <c r="W64" s="10"/>
-      <c r="X64" s="10"/>
-      <c r="Y64" s="10"/>
-      <c r="Z64" s="10"/>
-      <c r="AA64" s="10"/>
-      <c r="AB64" s="10"/>
-      <c r="AC64" s="10"/>
-      <c r="AD64" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE64" s="10"/>
-      <c r="AF64" s="10"/>
-      <c r="AG64" s="10"/>
-      <c r="AH64" s="10"/>
-      <c r="AI64" s="10"/>
-      <c r="AJ64" s="10"/>
-      <c r="AK64" s="10"/>
-      <c r="AL64" s="10"/>
-      <c r="AM64" s="10"/>
-      <c r="AN64" s="10"/>
-      <c r="AO64" s="10"/>
-      <c r="AP64" s="10"/>
-      <c r="AQ64" s="11"/>
+      <c r="AC64" s="7"/>
+      <c r="AD64" s="7"/>
+      <c r="AE64" s="7"/>
+      <c r="AF64" s="7"/>
+      <c r="AG64" s="7"/>
+      <c r="AH64" s="7"/>
+      <c r="AI64" s="7"/>
+      <c r="AJ64" s="7"/>
+      <c r="AK64" s="7"/>
+      <c r="AL64" s="7"/>
+      <c r="AM64" s="7"/>
+      <c r="AN64" s="7"/>
+      <c r="AO64" s="7"/>
+      <c r="AP64" s="7"/>
+      <c r="AQ64" s="8"/>
     </row>
     <row r="65" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C65" s="9"/>
-      <c r="D65" s="10"/>
+      <c r="D65" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
@@ -5046,10 +4679,10 @@
       <c r="Z65" s="10"/>
       <c r="AA65" s="10"/>
       <c r="AB65" s="10"/>
-      <c r="AC65" s="10"/>
-      <c r="AD65" s="10" t="s">
-        <v>27</v>
-      </c>
+      <c r="AC65" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD65" s="10"/>
       <c r="AE65" s="10"/>
       <c r="AF65" s="10"/>
       <c r="AG65" s="10"/>
@@ -5065,119 +4698,249 @@
       <c r="AQ65" s="11"/>
     </row>
     <row r="66" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C66" s="12"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="13"/>
-      <c r="R66" s="13"/>
-      <c r="S66" s="13"/>
-      <c r="T66" s="13"/>
-      <c r="U66" s="13"/>
-      <c r="V66" s="13"/>
-      <c r="W66" s="13"/>
-      <c r="X66" s="13"/>
-      <c r="Y66" s="13"/>
-      <c r="Z66" s="13"/>
-      <c r="AA66" s="13"/>
-      <c r="AB66" s="13"/>
-      <c r="AC66" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD66" s="13"/>
-      <c r="AE66" s="13"/>
-      <c r="AF66" s="13"/>
-      <c r="AG66" s="13"/>
-      <c r="AH66" s="13"/>
-      <c r="AI66" s="13"/>
-      <c r="AJ66" s="13"/>
-      <c r="AK66" s="13"/>
-      <c r="AL66" s="13"/>
-      <c r="AM66" s="13"/>
-      <c r="AN66" s="13"/>
-      <c r="AO66" s="13"/>
-      <c r="AP66" s="13"/>
-      <c r="AQ66" s="14"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
+      <c r="V66" s="10"/>
+      <c r="W66" s="10"/>
+      <c r="X66" s="10"/>
+      <c r="Y66" s="10"/>
+      <c r="Z66" s="10"/>
+      <c r="AA66" s="10"/>
+      <c r="AB66" s="10"/>
+      <c r="AC66" s="10"/>
+      <c r="AD66" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE66" s="10"/>
+      <c r="AF66" s="10"/>
+      <c r="AG66" s="10"/>
+      <c r="AH66" s="10"/>
+      <c r="AI66" s="10"/>
+      <c r="AJ66" s="10"/>
+      <c r="AK66" s="10"/>
+      <c r="AL66" s="10"/>
+      <c r="AM66" s="10"/>
+      <c r="AN66" s="10"/>
+      <c r="AO66" s="10"/>
+      <c r="AP66" s="10"/>
+      <c r="AQ66" s="11"/>
+    </row>
+    <row r="67" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C67" s="9"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
+      <c r="V67" s="10"/>
+      <c r="W67" s="10"/>
+      <c r="X67" s="10"/>
+      <c r="Y67" s="10"/>
+      <c r="Z67" s="10"/>
+      <c r="AA67" s="10"/>
+      <c r="AB67" s="10"/>
+      <c r="AC67" s="10"/>
+      <c r="AD67" s="10"/>
+      <c r="AE67" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF67" s="10"/>
+      <c r="AG67" s="10"/>
+      <c r="AH67" s="10"/>
+      <c r="AI67" s="10"/>
+      <c r="AJ67" s="10"/>
+      <c r="AK67" s="10"/>
+      <c r="AL67" s="10"/>
+      <c r="AM67" s="10"/>
+      <c r="AN67" s="10"/>
+      <c r="AO67" s="10"/>
+      <c r="AP67" s="10"/>
+      <c r="AQ67" s="11"/>
     </row>
     <row r="68" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C68" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="10"/>
+      <c r="V68" s="10"/>
+      <c r="W68" s="10"/>
+      <c r="X68" s="10"/>
+      <c r="Y68" s="10"/>
+      <c r="Z68" s="10"/>
+      <c r="AA68" s="10"/>
+      <c r="AB68" s="10"/>
+      <c r="AC68" s="10"/>
+      <c r="AD68" s="10"/>
+      <c r="AE68" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF68" s="10"/>
+      <c r="AG68" s="10"/>
+      <c r="AH68" s="10"/>
+      <c r="AI68" s="10"/>
+      <c r="AJ68" s="10"/>
+      <c r="AK68" s="10"/>
+      <c r="AL68" s="10"/>
+      <c r="AM68" s="10"/>
+      <c r="AN68" s="10"/>
+      <c r="AO68" s="10"/>
+      <c r="AP68" s="10"/>
+      <c r="AQ68" s="11"/>
     </row>
     <row r="69" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C69" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB69" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="10"/>
+      <c r="X69" s="10"/>
+      <c r="Y69" s="10"/>
+      <c r="Z69" s="10"/>
+      <c r="AA69" s="10"/>
+      <c r="AB69" s="10"/>
+      <c r="AC69" s="10"/>
+      <c r="AD69" s="10"/>
+      <c r="AE69" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF69" s="10"/>
+      <c r="AG69" s="10"/>
+      <c r="AH69" s="10"/>
+      <c r="AI69" s="10"/>
+      <c r="AJ69" s="10"/>
+      <c r="AK69" s="10"/>
+      <c r="AL69" s="10"/>
+      <c r="AM69" s="10"/>
+      <c r="AN69" s="10"/>
+      <c r="AO69" s="10"/>
+      <c r="AP69" s="10"/>
+      <c r="AQ69" s="11"/>
     </row>
     <row r="70" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C70" s="6"/>
-      <c r="D70" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-      <c r="P70" s="7"/>
-      <c r="Q70" s="7"/>
-      <c r="R70" s="7"/>
-      <c r="S70" s="7"/>
-      <c r="T70" s="7"/>
-      <c r="U70" s="7"/>
-      <c r="V70" s="7"/>
-      <c r="W70" s="7"/>
-      <c r="X70" s="7"/>
-      <c r="Y70" s="7"/>
-      <c r="Z70" s="7"/>
-      <c r="AA70" s="7"/>
-      <c r="AB70" s="7"/>
-      <c r="AC70" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD70" s="7"/>
-      <c r="AE70" s="7"/>
-      <c r="AF70" s="7"/>
-      <c r="AG70" s="7"/>
-      <c r="AH70" s="7"/>
-      <c r="AI70" s="7"/>
-      <c r="AJ70" s="7"/>
-      <c r="AK70" s="7"/>
-      <c r="AL70" s="7"/>
-      <c r="AM70" s="7"/>
-      <c r="AN70" s="7"/>
-      <c r="AO70" s="7"/>
-      <c r="AP70" s="7"/>
-      <c r="AQ70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="10"/>
+      <c r="V70" s="10"/>
+      <c r="W70" s="10"/>
+      <c r="X70" s="10"/>
+      <c r="Y70" s="10"/>
+      <c r="Z70" s="10"/>
+      <c r="AA70" s="10"/>
+      <c r="AB70" s="10"/>
+      <c r="AC70" s="10"/>
+      <c r="AD70" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE70" s="10"/>
+      <c r="AF70" s="10"/>
+      <c r="AG70" s="10"/>
+      <c r="AH70" s="10"/>
+      <c r="AI70" s="10"/>
+      <c r="AJ70" s="10"/>
+      <c r="AK70" s="10"/>
+      <c r="AL70" s="10"/>
+      <c r="AM70" s="10"/>
+      <c r="AN70" s="10"/>
+      <c r="AO70" s="10"/>
+      <c r="AP70" s="10"/>
+      <c r="AQ70" s="11"/>
     </row>
     <row r="71" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
-      <c r="E71" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="E71" s="10"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
+      <c r="H71" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
@@ -5219,12 +4982,12 @@
     <row r="72" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C72" s="9"/>
       <c r="D72" s="10"/>
-      <c r="E72" s="10" t="s">
-        <v>52</v>
-      </c>
+      <c r="E72" s="10"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
-      <c r="H72" s="10"/>
+      <c r="H72" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="I72" s="10"/>
       <c r="J72" s="10"/>
       <c r="K72" s="10"/>
@@ -5248,7 +5011,7 @@
       <c r="AC72" s="10"/>
       <c r="AD72" s="10"/>
       <c r="AE72" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="AF72" s="10"/>
       <c r="AG72" s="10"/>
@@ -5266,11 +5029,11 @@
     <row r="73" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C73" s="9"/>
       <c r="D73" s="10"/>
-      <c r="E73" s="10" t="s">
-        <v>36</v>
-      </c>
+      <c r="E73" s="10"/>
       <c r="F73" s="10"/>
-      <c r="G73" s="10"/>
+      <c r="G73" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
       <c r="J73" s="10"/>
@@ -5295,7 +5058,7 @@
       <c r="AC73" s="10"/>
       <c r="AD73" s="10"/>
       <c r="AE73" s="10" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="AF73" s="10"/>
       <c r="AG73" s="10"/>
@@ -5315,7 +5078,7 @@
       <c r="D74" s="10"/>
       <c r="E74" s="10"/>
       <c r="F74" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G74" s="10"/>
       <c r="H74" s="10"/>
@@ -5342,7 +5105,7 @@
       <c r="AC74" s="10"/>
       <c r="AD74" s="10"/>
       <c r="AE74" s="10" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="AF74" s="10"/>
       <c r="AG74" s="10"/>
@@ -5359,12 +5122,12 @@
     </row>
     <row r="75" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C75" s="9"/>
-      <c r="D75" s="10"/>
+      <c r="D75" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="E75" s="10"/>
       <c r="F75" s="10"/>
-      <c r="G75" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="G75" s="10"/>
       <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="10"/>
@@ -5387,10 +5150,10 @@
       <c r="AA75" s="10"/>
       <c r="AB75" s="10"/>
       <c r="AC75" s="10"/>
-      <c r="AD75" s="10"/>
-      <c r="AE75" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="AD75" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE75" s="10"/>
       <c r="AF75" s="10"/>
       <c r="AG75" s="10"/>
       <c r="AH75" s="10"/>
@@ -5410,9 +5173,7 @@
       <c r="E76" s="10"/>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
-      <c r="H76" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="H76" s="10"/>
       <c r="I76" s="10"/>
       <c r="J76" s="10"/>
       <c r="K76" s="10"/>
@@ -5434,10 +5195,10 @@
       <c r="AA76" s="10"/>
       <c r="AB76" s="10"/>
       <c r="AC76" s="10"/>
-      <c r="AD76" s="10"/>
-      <c r="AE76" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="AD76" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE76" s="10"/>
       <c r="AF76" s="10"/>
       <c r="AG76" s="10"/>
       <c r="AH76" s="10"/>
@@ -5452,248 +5213,118 @@
       <c r="AQ76" s="11"/>
     </row>
     <row r="77" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C77" s="9"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="10"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
-      <c r="H77" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I77" s="10"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-      <c r="L77" s="10"/>
-      <c r="M77" s="10"/>
-      <c r="N77" s="10"/>
-      <c r="O77" s="10"/>
-      <c r="P77" s="10"/>
-      <c r="Q77" s="10"/>
-      <c r="R77" s="10"/>
-      <c r="S77" s="10"/>
-      <c r="T77" s="10"/>
-      <c r="U77" s="10"/>
-      <c r="V77" s="10"/>
-      <c r="W77" s="10"/>
-      <c r="X77" s="10"/>
-      <c r="Y77" s="10"/>
-      <c r="Z77" s="10"/>
-      <c r="AA77" s="10"/>
-      <c r="AB77" s="10"/>
-      <c r="AC77" s="10"/>
-      <c r="AD77" s="10"/>
-      <c r="AE77" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF77" s="10"/>
-      <c r="AG77" s="10"/>
-      <c r="AH77" s="10"/>
-      <c r="AI77" s="10"/>
-      <c r="AJ77" s="10"/>
-      <c r="AK77" s="10"/>
-      <c r="AL77" s="10"/>
-      <c r="AM77" s="10"/>
-      <c r="AN77" s="10"/>
-      <c r="AO77" s="10"/>
-      <c r="AP77" s="10"/>
-      <c r="AQ77" s="11"/>
-    </row>
-    <row r="78" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C78" s="9"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
-      <c r="O78" s="10"/>
-      <c r="P78" s="10"/>
-      <c r="Q78" s="10"/>
-      <c r="R78" s="10"/>
-      <c r="S78" s="10"/>
-      <c r="T78" s="10"/>
-      <c r="U78" s="10"/>
-      <c r="V78" s="10"/>
-      <c r="W78" s="10"/>
-      <c r="X78" s="10"/>
-      <c r="Y78" s="10"/>
-      <c r="Z78" s="10"/>
-      <c r="AA78" s="10"/>
-      <c r="AB78" s="10"/>
-      <c r="AC78" s="10"/>
-      <c r="AD78" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE78" s="10"/>
-      <c r="AF78" s="10"/>
-      <c r="AG78" s="10"/>
-      <c r="AH78" s="10"/>
-      <c r="AI78" s="10"/>
-      <c r="AJ78" s="10"/>
-      <c r="AK78" s="10"/>
-      <c r="AL78" s="10"/>
-      <c r="AM78" s="10"/>
-      <c r="AN78" s="10"/>
-      <c r="AO78" s="10"/>
-      <c r="AP78" s="10"/>
-      <c r="AQ78" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="13"/>
+      <c r="L77" s="13"/>
+      <c r="M77" s="13"/>
+      <c r="N77" s="13"/>
+      <c r="O77" s="13"/>
+      <c r="P77" s="13"/>
+      <c r="Q77" s="13"/>
+      <c r="R77" s="13"/>
+      <c r="S77" s="13"/>
+      <c r="T77" s="13"/>
+      <c r="U77" s="13"/>
+      <c r="V77" s="13"/>
+      <c r="W77" s="13"/>
+      <c r="X77" s="13"/>
+      <c r="Y77" s="13"/>
+      <c r="Z77" s="13"/>
+      <c r="AA77" s="13"/>
+      <c r="AB77" s="13"/>
+      <c r="AC77" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD77" s="13"/>
+      <c r="AE77" s="13"/>
+      <c r="AF77" s="13"/>
+      <c r="AG77" s="13"/>
+      <c r="AH77" s="13"/>
+      <c r="AI77" s="13"/>
+      <c r="AJ77" s="13"/>
+      <c r="AK77" s="13"/>
+      <c r="AL77" s="13"/>
+      <c r="AM77" s="13"/>
+      <c r="AN77" s="13"/>
+      <c r="AO77" s="13"/>
+      <c r="AP77" s="13"/>
+      <c r="AQ77" s="14"/>
     </row>
     <row r="79" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C79" s="9"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="10"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H79" s="10"/>
-      <c r="I79" s="10"/>
-      <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10"/>
-      <c r="O79" s="10"/>
-      <c r="P79" s="10"/>
-      <c r="Q79" s="10"/>
-      <c r="R79" s="10"/>
-      <c r="S79" s="10"/>
-      <c r="T79" s="10"/>
-      <c r="U79" s="10"/>
-      <c r="V79" s="10"/>
-      <c r="W79" s="10"/>
-      <c r="X79" s="10"/>
-      <c r="Y79" s="10"/>
-      <c r="Z79" s="10"/>
-      <c r="AA79" s="10"/>
-      <c r="AB79" s="10"/>
-      <c r="AC79" s="10"/>
-      <c r="AD79" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE79" s="10"/>
-      <c r="AF79" s="10"/>
-      <c r="AG79" s="10"/>
-      <c r="AH79" s="10"/>
-      <c r="AI79" s="10"/>
-      <c r="AJ79" s="10"/>
-      <c r="AK79" s="10"/>
-      <c r="AL79" s="10"/>
-      <c r="AM79" s="10"/>
-      <c r="AN79" s="10"/>
-      <c r="AO79" s="10"/>
-      <c r="AP79" s="10"/>
-      <c r="AQ79" s="11"/>
+      <c r="C79" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="80" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C80" s="9"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="10"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
-      <c r="H80" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I80" s="10"/>
-      <c r="J80" s="10"/>
-      <c r="K80" s="10"/>
-      <c r="L80" s="10"/>
-      <c r="M80" s="10"/>
-      <c r="N80" s="10"/>
-      <c r="O80" s="10"/>
-      <c r="P80" s="10"/>
-      <c r="Q80" s="10"/>
-      <c r="R80" s="10"/>
-      <c r="S80" s="10"/>
-      <c r="T80" s="10"/>
-      <c r="U80" s="10"/>
-      <c r="V80" s="10"/>
-      <c r="W80" s="10"/>
-      <c r="X80" s="10"/>
-      <c r="Y80" s="10"/>
-      <c r="Z80" s="10"/>
-      <c r="AA80" s="10"/>
-      <c r="AB80" s="10"/>
-      <c r="AC80" s="10"/>
-      <c r="AD80" s="10"/>
-      <c r="AE80" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF80" s="10"/>
-      <c r="AG80" s="10"/>
-      <c r="AH80" s="10"/>
-      <c r="AI80" s="10"/>
-      <c r="AJ80" s="10"/>
-      <c r="AK80" s="10"/>
-      <c r="AL80" s="10"/>
-      <c r="AM80" s="10"/>
-      <c r="AN80" s="10"/>
-      <c r="AO80" s="10"/>
-      <c r="AP80" s="10"/>
-      <c r="AQ80" s="11"/>
+      <c r="C80" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB80" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="81" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C81" s="9"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="I81" s="10"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10"/>
-      <c r="O81" s="10"/>
-      <c r="P81" s="10"/>
-      <c r="Q81" s="10"/>
-      <c r="R81" s="10"/>
-      <c r="S81" s="10"/>
-      <c r="T81" s="10"/>
-      <c r="U81" s="10"/>
-      <c r="V81" s="10"/>
-      <c r="W81" s="10"/>
-      <c r="X81" s="10"/>
-      <c r="Y81" s="10"/>
-      <c r="Z81" s="10"/>
-      <c r="AA81" s="10"/>
-      <c r="AB81" s="10"/>
-      <c r="AC81" s="10"/>
-      <c r="AD81" s="10"/>
-      <c r="AE81" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF81" s="10"/>
-      <c r="AG81" s="10"/>
-      <c r="AH81" s="10"/>
-      <c r="AI81" s="10"/>
-      <c r="AJ81" s="10"/>
-      <c r="AK81" s="10"/>
-      <c r="AL81" s="10"/>
-      <c r="AM81" s="10"/>
-      <c r="AN81" s="10"/>
-      <c r="AO81" s="10"/>
-      <c r="AP81" s="10"/>
-      <c r="AQ81" s="11"/>
+      <c r="C81" s="6"/>
+      <c r="D81" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7"/>
+      <c r="AC81" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7"/>
+      <c r="AL81" s="7"/>
+      <c r="AM81" s="7"/>
+      <c r="AN81" s="7"/>
+      <c r="AO81" s="7"/>
+      <c r="AP81" s="7"/>
+      <c r="AQ81" s="8"/>
     </row>
     <row r="82" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C82" s="9"/>
       <c r="D82" s="10"/>
-      <c r="E82" s="10"/>
+      <c r="E82" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="F82" s="10"/>
-      <c r="G82" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="G82" s="10"/>
       <c r="H82" s="10"/>
       <c r="I82" s="10"/>
       <c r="J82" s="10"/>
@@ -5716,10 +5347,10 @@
       <c r="AA82" s="10"/>
       <c r="AB82" s="10"/>
       <c r="AC82" s="10"/>
-      <c r="AD82" s="10"/>
-      <c r="AE82" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="AD82" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE82" s="10"/>
       <c r="AF82" s="10"/>
       <c r="AG82" s="10"/>
       <c r="AH82" s="10"/>
@@ -5736,11 +5367,11 @@
     <row r="83" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="10"/>
+      <c r="E83" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="F83" s="10"/>
-      <c r="G83" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="G83" s="10"/>
       <c r="H83" s="10"/>
       <c r="I83" s="10"/>
       <c r="J83" s="10"/>
@@ -5765,7 +5396,7 @@
       <c r="AC83" s="10"/>
       <c r="AD83" s="10"/>
       <c r="AE83" s="10" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="AF83" s="10"/>
       <c r="AG83" s="10"/>
@@ -5783,12 +5414,12 @@
     <row r="84" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
-      <c r="E84" s="10"/>
+      <c r="E84" s="10" t="s">
+        <v>36</v>
+      </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
-      <c r="H84" s="10" t="s">
-        <v>56</v>
-      </c>
+      <c r="H84" s="10"/>
       <c r="I84" s="10"/>
       <c r="J84" s="10"/>
       <c r="K84" s="10"/>
@@ -5812,7 +5443,7 @@
       <c r="AC84" s="10"/>
       <c r="AD84" s="10"/>
       <c r="AE84" s="10" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="AF84" s="10"/>
       <c r="AG84" s="10"/>
@@ -5831,11 +5462,11 @@
       <c r="C85" s="9"/>
       <c r="D85" s="10"/>
       <c r="E85" s="10"/>
-      <c r="F85" s="10"/>
+      <c r="F85" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="G85" s="10"/>
-      <c r="H85" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="H85" s="10"/>
       <c r="I85" s="10"/>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -5859,7 +5490,7 @@
       <c r="AC85" s="10"/>
       <c r="AD85" s="10"/>
       <c r="AE85" s="10" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="AF85" s="10"/>
       <c r="AG85" s="10"/>
@@ -5880,7 +5511,7 @@
       <c r="E86" s="10"/>
       <c r="F86" s="10"/>
       <c r="G86" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H86" s="10"/>
       <c r="I86" s="10"/>
@@ -5904,10 +5535,10 @@
       <c r="AA86" s="10"/>
       <c r="AB86" s="10"/>
       <c r="AC86" s="10"/>
-      <c r="AD86" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE86" s="10"/>
+      <c r="AD86" s="10"/>
+      <c r="AE86" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="AF86" s="10"/>
       <c r="AG86" s="10"/>
       <c r="AH86" s="10"/>
@@ -5926,10 +5557,10 @@
       <c r="D87" s="10"/>
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
-      <c r="G87" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="I87" s="10"/>
       <c r="J87" s="10"/>
       <c r="K87" s="10"/>
@@ -5950,11 +5581,11 @@
       <c r="Z87" s="10"/>
       <c r="AA87" s="10"/>
       <c r="AB87" s="10"/>
-      <c r="AC87" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="AC87" s="10"/>
       <c r="AD87" s="10"/>
-      <c r="AE87" s="10"/>
+      <c r="AE87" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="AF87" s="10"/>
       <c r="AG87" s="10"/>
       <c r="AH87" s="10"/>
@@ -5972,11 +5603,11 @@
       <c r="C88" s="9"/>
       <c r="D88" s="10"/>
       <c r="E88" s="10"/>
-      <c r="F88" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F88" s="10"/>
       <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
+      <c r="H88" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="I88" s="10"/>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -5999,7 +5630,9 @@
       <c r="AB88" s="10"/>
       <c r="AC88" s="10"/>
       <c r="AD88" s="10"/>
-      <c r="AE88" s="10"/>
+      <c r="AE88" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="AF88" s="10"/>
       <c r="AG88" s="10"/>
       <c r="AH88" s="10"/>
@@ -6014,49 +5647,564 @@
       <c r="AQ88" s="11"/>
     </row>
     <row r="89" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C89" s="12"/>
-      <c r="D89" s="13" t="s">
+      <c r="C89" s="9"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
+      <c r="V89" s="10"/>
+      <c r="W89" s="10"/>
+      <c r="X89" s="10"/>
+      <c r="Y89" s="10"/>
+      <c r="Z89" s="10"/>
+      <c r="AA89" s="10"/>
+      <c r="AB89" s="10"/>
+      <c r="AC89" s="10"/>
+      <c r="AD89" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE89" s="10"/>
+      <c r="AF89" s="10"/>
+      <c r="AG89" s="10"/>
+      <c r="AH89" s="10"/>
+      <c r="AI89" s="10"/>
+      <c r="AJ89" s="10"/>
+      <c r="AK89" s="10"/>
+      <c r="AL89" s="10"/>
+      <c r="AM89" s="10"/>
+      <c r="AN89" s="10"/>
+      <c r="AO89" s="10"/>
+      <c r="AP89" s="10"/>
+      <c r="AQ89" s="11"/>
+    </row>
+    <row r="90" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C90" s="9"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
+      <c r="V90" s="10"/>
+      <c r="W90" s="10"/>
+      <c r="X90" s="10"/>
+      <c r="Y90" s="10"/>
+      <c r="Z90" s="10"/>
+      <c r="AA90" s="10"/>
+      <c r="AB90" s="10"/>
+      <c r="AC90" s="10"/>
+      <c r="AD90" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE90" s="10"/>
+      <c r="AF90" s="10"/>
+      <c r="AG90" s="10"/>
+      <c r="AH90" s="10"/>
+      <c r="AI90" s="10"/>
+      <c r="AJ90" s="10"/>
+      <c r="AK90" s="10"/>
+      <c r="AL90" s="10"/>
+      <c r="AM90" s="10"/>
+      <c r="AN90" s="10"/>
+      <c r="AO90" s="10"/>
+      <c r="AP90" s="10"/>
+      <c r="AQ90" s="11"/>
+    </row>
+    <row r="91" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C91" s="9"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10"/>
+      <c r="V91" s="10"/>
+      <c r="W91" s="10"/>
+      <c r="X91" s="10"/>
+      <c r="Y91" s="10"/>
+      <c r="Z91" s="10"/>
+      <c r="AA91" s="10"/>
+      <c r="AB91" s="10"/>
+      <c r="AC91" s="10"/>
+      <c r="AD91" s="10"/>
+      <c r="AE91" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF91" s="10"/>
+      <c r="AG91" s="10"/>
+      <c r="AH91" s="10"/>
+      <c r="AI91" s="10"/>
+      <c r="AJ91" s="10"/>
+      <c r="AK91" s="10"/>
+      <c r="AL91" s="10"/>
+      <c r="AM91" s="10"/>
+      <c r="AN91" s="10"/>
+      <c r="AO91" s="10"/>
+      <c r="AP91" s="10"/>
+      <c r="AQ91" s="11"/>
+    </row>
+    <row r="92" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C92" s="9"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
+      <c r="N92" s="10"/>
+      <c r="O92" s="10"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+      <c r="S92" s="10"/>
+      <c r="T92" s="10"/>
+      <c r="U92" s="10"/>
+      <c r="V92" s="10"/>
+      <c r="W92" s="10"/>
+      <c r="X92" s="10"/>
+      <c r="Y92" s="10"/>
+      <c r="Z92" s="10"/>
+      <c r="AA92" s="10"/>
+      <c r="AB92" s="10"/>
+      <c r="AC92" s="10"/>
+      <c r="AD92" s="10"/>
+      <c r="AE92" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF92" s="10"/>
+      <c r="AG92" s="10"/>
+      <c r="AH92" s="10"/>
+      <c r="AI92" s="10"/>
+      <c r="AJ92" s="10"/>
+      <c r="AK92" s="10"/>
+      <c r="AL92" s="10"/>
+      <c r="AM92" s="10"/>
+      <c r="AN92" s="10"/>
+      <c r="AO92" s="10"/>
+      <c r="AP92" s="10"/>
+      <c r="AQ92" s="11"/>
+    </row>
+    <row r="93" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C93" s="9"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="10"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
+      <c r="U93" s="10"/>
+      <c r="V93" s="10"/>
+      <c r="W93" s="10"/>
+      <c r="X93" s="10"/>
+      <c r="Y93" s="10"/>
+      <c r="Z93" s="10"/>
+      <c r="AA93" s="10"/>
+      <c r="AB93" s="10"/>
+      <c r="AC93" s="10"/>
+      <c r="AD93" s="10"/>
+      <c r="AE93" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF93" s="10"/>
+      <c r="AG93" s="10"/>
+      <c r="AH93" s="10"/>
+      <c r="AI93" s="10"/>
+      <c r="AJ93" s="10"/>
+      <c r="AK93" s="10"/>
+      <c r="AL93" s="10"/>
+      <c r="AM93" s="10"/>
+      <c r="AN93" s="10"/>
+      <c r="AO93" s="10"/>
+      <c r="AP93" s="10"/>
+      <c r="AQ93" s="11"/>
+    </row>
+    <row r="94" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C94" s="9"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="10"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
+      <c r="U94" s="10"/>
+      <c r="V94" s="10"/>
+      <c r="W94" s="10"/>
+      <c r="X94" s="10"/>
+      <c r="Y94" s="10"/>
+      <c r="Z94" s="10"/>
+      <c r="AA94" s="10"/>
+      <c r="AB94" s="10"/>
+      <c r="AC94" s="10"/>
+      <c r="AD94" s="10"/>
+      <c r="AE94" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF94" s="10"/>
+      <c r="AG94" s="10"/>
+      <c r="AH94" s="10"/>
+      <c r="AI94" s="10"/>
+      <c r="AJ94" s="10"/>
+      <c r="AK94" s="10"/>
+      <c r="AL94" s="10"/>
+      <c r="AM94" s="10"/>
+      <c r="AN94" s="10"/>
+      <c r="AO94" s="10"/>
+      <c r="AP94" s="10"/>
+      <c r="AQ94" s="11"/>
+    </row>
+    <row r="95" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C95" s="9"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
+      <c r="N95" s="10"/>
+      <c r="O95" s="10"/>
+      <c r="P95" s="10"/>
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10"/>
+      <c r="S95" s="10"/>
+      <c r="T95" s="10"/>
+      <c r="U95" s="10"/>
+      <c r="V95" s="10"/>
+      <c r="W95" s="10"/>
+      <c r="X95" s="10"/>
+      <c r="Y95" s="10"/>
+      <c r="Z95" s="10"/>
+      <c r="AA95" s="10"/>
+      <c r="AB95" s="10"/>
+      <c r="AC95" s="10"/>
+      <c r="AD95" s="10"/>
+      <c r="AE95" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF95" s="10"/>
+      <c r="AG95" s="10"/>
+      <c r="AH95" s="10"/>
+      <c r="AI95" s="10"/>
+      <c r="AJ95" s="10"/>
+      <c r="AK95" s="10"/>
+      <c r="AL95" s="10"/>
+      <c r="AM95" s="10"/>
+      <c r="AN95" s="10"/>
+      <c r="AO95" s="10"/>
+      <c r="AP95" s="10"/>
+      <c r="AQ95" s="11"/>
+    </row>
+    <row r="96" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C96" s="9"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+      <c r="M96" s="10"/>
+      <c r="N96" s="10"/>
+      <c r="O96" s="10"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="10"/>
+      <c r="R96" s="10"/>
+      <c r="S96" s="10"/>
+      <c r="T96" s="10"/>
+      <c r="U96" s="10"/>
+      <c r="V96" s="10"/>
+      <c r="W96" s="10"/>
+      <c r="X96" s="10"/>
+      <c r="Y96" s="10"/>
+      <c r="Z96" s="10"/>
+      <c r="AA96" s="10"/>
+      <c r="AB96" s="10"/>
+      <c r="AC96" s="10"/>
+      <c r="AD96" s="10"/>
+      <c r="AE96" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF96" s="10"/>
+      <c r="AG96" s="10"/>
+      <c r="AH96" s="10"/>
+      <c r="AI96" s="10"/>
+      <c r="AJ96" s="10"/>
+      <c r="AK96" s="10"/>
+      <c r="AL96" s="10"/>
+      <c r="AM96" s="10"/>
+      <c r="AN96" s="10"/>
+      <c r="AO96" s="10"/>
+      <c r="AP96" s="10"/>
+      <c r="AQ96" s="11"/>
+    </row>
+    <row r="97" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C97" s="9"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
+      <c r="L97" s="10"/>
+      <c r="M97" s="10"/>
+      <c r="N97" s="10"/>
+      <c r="O97" s="10"/>
+      <c r="P97" s="10"/>
+      <c r="Q97" s="10"/>
+      <c r="R97" s="10"/>
+      <c r="S97" s="10"/>
+      <c r="T97" s="10"/>
+      <c r="U97" s="10"/>
+      <c r="V97" s="10"/>
+      <c r="W97" s="10"/>
+      <c r="X97" s="10"/>
+      <c r="Y97" s="10"/>
+      <c r="Z97" s="10"/>
+      <c r="AA97" s="10"/>
+      <c r="AB97" s="10"/>
+      <c r="AC97" s="10"/>
+      <c r="AD97" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE97" s="10"/>
+      <c r="AF97" s="10"/>
+      <c r="AG97" s="10"/>
+      <c r="AH97" s="10"/>
+      <c r="AI97" s="10"/>
+      <c r="AJ97" s="10"/>
+      <c r="AK97" s="10"/>
+      <c r="AL97" s="10"/>
+      <c r="AM97" s="10"/>
+      <c r="AN97" s="10"/>
+      <c r="AO97" s="10"/>
+      <c r="AP97" s="10"/>
+      <c r="AQ97" s="11"/>
+    </row>
+    <row r="98" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C98" s="9"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10"/>
+      <c r="K98" s="10"/>
+      <c r="L98" s="10"/>
+      <c r="M98" s="10"/>
+      <c r="N98" s="10"/>
+      <c r="O98" s="10"/>
+      <c r="P98" s="10"/>
+      <c r="Q98" s="10"/>
+      <c r="R98" s="10"/>
+      <c r="S98" s="10"/>
+      <c r="T98" s="10"/>
+      <c r="U98" s="10"/>
+      <c r="V98" s="10"/>
+      <c r="W98" s="10"/>
+      <c r="X98" s="10"/>
+      <c r="Y98" s="10"/>
+      <c r="Z98" s="10"/>
+      <c r="AA98" s="10"/>
+      <c r="AB98" s="10"/>
+      <c r="AC98" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="13"/>
-      <c r="N89" s="13"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
-      <c r="S89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="13"/>
-      <c r="W89" s="13"/>
-      <c r="X89" s="13"/>
-      <c r="Y89" s="13"/>
-      <c r="Z89" s="13"/>
-      <c r="AA89" s="13"/>
-      <c r="AB89" s="13"/>
-      <c r="AC89" s="13"/>
-      <c r="AD89" s="13"/>
-      <c r="AE89" s="13"/>
-      <c r="AF89" s="13"/>
-      <c r="AG89" s="13"/>
-      <c r="AH89" s="13"/>
-      <c r="AI89" s="13"/>
-      <c r="AJ89" s="13"/>
-      <c r="AK89" s="13"/>
-      <c r="AL89" s="13"/>
-      <c r="AM89" s="13"/>
-      <c r="AN89" s="13"/>
-      <c r="AO89" s="13"/>
-      <c r="AP89" s="13"/>
-      <c r="AQ89" s="14"/>
+      <c r="AD98" s="10"/>
+      <c r="AE98" s="10"/>
+      <c r="AF98" s="10"/>
+      <c r="AG98" s="10"/>
+      <c r="AH98" s="10"/>
+      <c r="AI98" s="10"/>
+      <c r="AJ98" s="10"/>
+      <c r="AK98" s="10"/>
+      <c r="AL98" s="10"/>
+      <c r="AM98" s="10"/>
+      <c r="AN98" s="10"/>
+      <c r="AO98" s="10"/>
+      <c r="AP98" s="10"/>
+      <c r="AQ98" s="11"/>
+    </row>
+    <row r="99" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C99" s="9"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="10"/>
+      <c r="L99" s="10"/>
+      <c r="M99" s="10"/>
+      <c r="N99" s="10"/>
+      <c r="O99" s="10"/>
+      <c r="P99" s="10"/>
+      <c r="Q99" s="10"/>
+      <c r="R99" s="10"/>
+      <c r="S99" s="10"/>
+      <c r="T99" s="10"/>
+      <c r="U99" s="10"/>
+      <c r="V99" s="10"/>
+      <c r="W99" s="10"/>
+      <c r="X99" s="10"/>
+      <c r="Y99" s="10"/>
+      <c r="Z99" s="10"/>
+      <c r="AA99" s="10"/>
+      <c r="AB99" s="10"/>
+      <c r="AC99" s="10"/>
+      <c r="AD99" s="10"/>
+      <c r="AE99" s="10"/>
+      <c r="AF99" s="10"/>
+      <c r="AG99" s="10"/>
+      <c r="AH99" s="10"/>
+      <c r="AI99" s="10"/>
+      <c r="AJ99" s="10"/>
+      <c r="AK99" s="10"/>
+      <c r="AL99" s="10"/>
+      <c r="AM99" s="10"/>
+      <c r="AN99" s="10"/>
+      <c r="AO99" s="10"/>
+      <c r="AP99" s="10"/>
+      <c r="AQ99" s="11"/>
+    </row>
+    <row r="100" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C100" s="12"/>
+      <c r="D100" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="13"/>
+      <c r="K100" s="13"/>
+      <c r="L100" s="13"/>
+      <c r="M100" s="13"/>
+      <c r="N100" s="13"/>
+      <c r="O100" s="13"/>
+      <c r="P100" s="13"/>
+      <c r="Q100" s="13"/>
+      <c r="R100" s="13"/>
+      <c r="S100" s="13"/>
+      <c r="T100" s="13"/>
+      <c r="U100" s="13"/>
+      <c r="V100" s="13"/>
+      <c r="W100" s="13"/>
+      <c r="X100" s="13"/>
+      <c r="Y100" s="13"/>
+      <c r="Z100" s="13"/>
+      <c r="AA100" s="13"/>
+      <c r="AB100" s="13"/>
+      <c r="AC100" s="13"/>
+      <c r="AD100" s="13"/>
+      <c r="AE100" s="13"/>
+      <c r="AF100" s="13"/>
+      <c r="AG100" s="13"/>
+      <c r="AH100" s="13"/>
+      <c r="AI100" s="13"/>
+      <c r="AJ100" s="13"/>
+      <c r="AK100" s="13"/>
+      <c r="AL100" s="13"/>
+      <c r="AM100" s="13"/>
+      <c r="AN100" s="13"/>
+      <c r="AO100" s="13"/>
+      <c r="AP100" s="13"/>
+      <c r="AQ100" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add LightGBM model training using California Housing dataset
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13110" windowHeight="9075" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="10470" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="158">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -625,6 +625,14 @@
   </si>
   <si>
     <t>// value list for select</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"learning_rate": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// learning rate (configurable)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6513,10 +6521,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T52"/>
+  <dimension ref="B2:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6729,139 +6737,147 @@
     </row>
     <row r="31" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E31" s="15" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E32" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T32" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E33" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T33" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E34" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="T34" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E35" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="T34" s="15" t="s">
+      <c r="T35" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D35" s="15" t="s">
+    <row r="36" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D36" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C36" s="15" t="s">
+    <row r="37" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C37" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="16" t="s">
+    <row r="39" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39" s="16" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C39" s="15" t="s">
+    <row r="40" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C40" s="15" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D40" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="T40" s="15" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="41" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D41" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T41" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D42" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T42" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D43" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T43" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D44" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="T44" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D45" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="T44" s="15" t="s">
+      <c r="T45" s="15" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E45" s="15" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="46" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E46" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E47" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D47" s="15" t="s">
+    <row r="48" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D48" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T47" s="15" t="s">
+      <c r="T48" s="15" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E48" s="15" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="49" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E49" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E50" s="15" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D50" s="15" t="s">
+    <row r="51" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D51" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="T50" s="15" t="s">
+      <c r="T51" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E51" s="15" t="s">
+    <row r="52" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E52" s="15" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C52" s="15" t="s">
+    <row r="53" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C53" s="15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update MLP model training (add parameter about MLP structure)
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="10470" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="182">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -709,6 +709,26 @@
   </si>
   <si>
     <t>// bagging fraction (configurable)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"mlp_structure": {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>},</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"num_of_hidden_nodes": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// structure parameters (show on MLP model only)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// number of hidden nodes (configurable)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6597,10 +6617,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T64"/>
+  <dimension ref="B2:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6789,256 +6809,277 @@
     </row>
     <row r="28" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D28" s="15" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="T28" s="15" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E29" s="15" t="s">
-        <v>103</v>
+        <v>179</v>
       </c>
       <c r="T29" s="15" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E30" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="T30" s="15" t="s">
-        <v>137</v>
+      <c r="D30" s="15" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E31" s="15" t="s">
-        <v>149</v>
+      <c r="D31" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="T31" s="15" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E32" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="T32" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E33" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="T33" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E34" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="T34" s="15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E35" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="T32" s="15" t="s">
+      <c r="T35" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E33" s="15" t="s">
+    <row r="36" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E36" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="T33" s="15" t="s">
+      <c r="T36" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E34" s="15" t="s">
+    <row r="37" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E37" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="T34" s="15" t="s">
+      <c r="T37" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E35" s="15" t="s">
+    <row r="38" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E38" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="T35" s="15" t="s">
+      <c r="T38" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D36" s="15" t="s">
+    <row r="39" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D39" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D37" s="15" t="s">
+    <row r="40" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D40" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="T37" s="15" t="s">
+      <c r="T40" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="38" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E38" s="15" t="s">
+    <row r="41" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E41" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="T38" s="15" t="s">
+      <c r="T41" s="15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="39" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E39" s="15" t="s">
+    <row r="42" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E42" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="T39" s="15" t="s">
+      <c r="T42" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E40" s="15" t="s">
+    <row r="43" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E43" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="T40" s="15" t="s">
+      <c r="T43" s="15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E41" s="15" t="s">
+    <row r="44" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E44" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="T41" s="15" t="s">
+      <c r="T44" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E42" s="15" t="s">
+    <row r="45" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E45" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="T42" s="15" t="s">
+      <c r="T45" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E43" s="15" t="s">
+    <row r="46" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E46" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="T43" s="15" t="s">
+      <c r="T46" s="15" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="44" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E44" s="15" t="s">
+    <row r="47" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E47" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="T44" s="15" t="s">
+      <c r="T47" s="15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E45" s="15" t="s">
+    <row r="48" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E48" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="T45" s="15" t="s">
+      <c r="T48" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="46" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E46" s="15" t="s">
+    <row r="49" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E49" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="T46" s="15" t="s">
+      <c r="T49" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="47" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D47" s="15" t="s">
+    <row r="50" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D50" s="15" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C48" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="16" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="51" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C51" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B53" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C54" s="15" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="52" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D52" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="T52" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D53" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="T53" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D54" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="T54" s="15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="55" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D55" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="T55" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D56" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="T56" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E57" s="15" t="s">
-        <v>127</v>
+      <c r="D57" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="T57" s="15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E58" s="15" t="s">
-        <v>128</v>
+      <c r="D58" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="T58" s="15" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D59" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T59" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E60" s="15" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E61" s="15" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D62" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="T62" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E63" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E64" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D65" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="T65" s="15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E66" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C64" s="15" t="s">
+    <row r="67" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C67" s="15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
streaming for trained model with AI Dashboard
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="10470" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21990" windowHeight="10320" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="196">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -729,6 +729,62 @@
   </si>
   <si>
     <t>// number of hidden nodes (configurable)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"inference_parameter": {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// inference parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>},</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"norm_coef_a": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"norm_coef_b": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"input_shape": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"preprocessing": {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// preprocessing parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// coeffiecient of normalization (y = (x-norm_coef_a) / norm_coef_b)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// input shape to AI model</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>},</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"task": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// model parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// task</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6617,10 +6673,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T67"/>
+  <dimension ref="B2:T77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="T59" sqref="T59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6983,103 +7039,174 @@
       </c>
     </row>
     <row r="51" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C51" s="15" t="s">
+      <c r="D51" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="T51" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E52" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="T52" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F53" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="T53" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F54" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="T54" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F55" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="T55" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E56" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E57" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="T57" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F58" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="T58" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E59" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D60" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B53" s="16" t="s">
+    <row r="61" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C61" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B63" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C54" s="15" t="s">
+    <row r="64" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C64" s="15" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D55" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="T55" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D56" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="T56" s="15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D57" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="T57" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="58" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D58" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="T58" s="15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D59" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="T59" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E60" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E61" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D62" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="T62" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E63" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E64" s="15" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="65" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D65" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="T65" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D66" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="T66" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D67" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="T67" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D68" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="T68" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D69" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="T69" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E70" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E71" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D72" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="T72" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E73" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E74" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="75" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D75" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T65" s="15" t="s">
+      <c r="T75" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E66" s="15" t="s">
+    <row r="76" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E76" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C67" s="15" t="s">
+    <row r="77" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C77" s="15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save input and output tensor name to config.json
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="200">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -785,6 +785,22 @@
   </si>
   <si>
     <t>// task</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"input_tensor_name": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"output_tensor_name": &lt;parameter block&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// input tensor name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// output tensor name</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -6673,10 +6689,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:T77"/>
+  <dimension ref="B2:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="T59" sqref="T59"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6859,354 +6875,370 @@
       </c>
     </row>
     <row r="27" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D27" s="15" t="s">
+      <c r="E27" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="T27" s="15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E28" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="T28" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D29" s="15" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D28" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="T28" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E29" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="T29" s="15" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="30" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D30" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="T30" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E31" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="T31" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D32" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="31" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D31" s="15" t="s">
+    <row r="33" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D33" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="T31" s="15" t="s">
+      <c r="T33" s="15" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E32" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="T32" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E33" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="T33" s="15" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="34" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E34" s="15" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
       <c r="T34" s="15" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E35" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="T35" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E36" s="15" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="T36" s="15" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E37" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="T37" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E38" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="T38" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E39" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="T39" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E40" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="T38" s="15" t="s">
+      <c r="T40" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D39" s="15" t="s">
+    <row r="41" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D41" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D40" s="15" t="s">
+    <row r="42" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D42" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="T40" s="15" t="s">
+      <c r="T42" s="15" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="41" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E41" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="T41" s="15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="42" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E42" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="T42" s="15" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="43" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E43" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="T43" s="15" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E44" s="15" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="T44" s="15" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E45" s="15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="T45" s="15" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E46" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T46" s="15" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E47" s="15" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="T47" s="15" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E48" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="T48" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E49" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="T49" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E50" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="T48" s="15" t="s">
+      <c r="T50" s="15" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="49" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E49" s="15" t="s">
+    <row r="51" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E51" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="T49" s="15" t="s">
+      <c r="T51" s="15" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D50" s="15" t="s">
+    <row r="52" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D52" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D51" s="15" t="s">
+    <row r="53" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D53" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="T51" s="15" t="s">
+      <c r="T53" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="52" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E52" s="15" t="s">
+    <row r="54" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E54" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="T52" s="15" t="s">
+      <c r="T54" s="15" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="53" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F53" s="15" t="s">
+    <row r="55" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F55" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="T53" s="15" t="s">
+      <c r="T55" s="15" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="54" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F54" s="15" t="s">
+    <row r="56" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F56" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="T54" s="15" t="s">
+      <c r="T56" s="15" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="55" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F55" s="15" t="s">
+    <row r="57" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F57" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="T55" s="15" t="s">
+      <c r="T57" s="15" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="56" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E56" s="15" t="s">
+    <row r="58" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E58" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="57" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E57" s="15" t="s">
+    <row r="59" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E59" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="T57" s="15" t="s">
+      <c r="T59" s="15" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="58" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="F58" s="15" t="s">
+    <row r="60" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="F60" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="T58" s="15" t="s">
+      <c r="T60" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E59" s="15" t="s">
+    <row r="61" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E61" s="15" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D60" s="15" t="s">
+    <row r="62" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D62" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C61" s="15" t="s">
+    <row r="63" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C63" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B63" s="16" t="s">
+    <row r="65" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C64" s="15" t="s">
+    <row r="66" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C66" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D65" s="15" t="s">
+    <row r="67" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D67" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="T65" s="15" t="s">
+      <c r="T67" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D66" s="15" t="s">
+    <row r="68" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D68" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="T66" s="15" t="s">
+      <c r="T68" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="67" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D67" s="15" t="s">
+    <row r="69" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D69" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="T67" s="15" t="s">
+      <c r="T69" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D68" s="15" t="s">
+    <row r="70" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D70" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="T68" s="15" t="s">
+      <c r="T70" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D69" s="15" t="s">
+    <row r="71" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D71" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="T69" s="15" t="s">
+      <c r="T71" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E70" s="15" t="s">
+    <row r="72" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E72" s="15" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E71" s="15" t="s">
+    <row r="73" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E73" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D72" s="15" t="s">
+    <row r="74" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D74" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="T72" s="15" t="s">
+      <c r="T74" s="15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E73" s="15" t="s">
+    <row r="75" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E75" s="15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E74" s="15" t="s">
+    <row r="76" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E76" s="15" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D75" s="15" t="s">
+    <row r="77" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D77" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="T75" s="15" t="s">
+      <c r="T77" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="76" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E76" s="15" t="s">
+    <row r="78" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E78" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C77" s="15" t="s">
+    <row r="79" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C79" s="15" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save info.json for COCO Dataset (base environment)
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21990" windowHeight="10320" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25965" windowHeight="10320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="218">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -179,10 +179,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>"task": &lt;"classification" or "regression"&gt;,</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&lt;key name&gt;: &lt;value&gt;,</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -323,10 +319,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>specifies the target value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>*1: if "type" is set to "image_file", please set to "img_file" to "name" field</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -802,6 +794,77 @@
   <si>
     <t>// output tensor name</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"task": &lt;"classification", "object_detection" or "regression"&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>specifies the target value (scalar or dict)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>example (object detection)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"task": "object_detection",</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"target": {</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"class_id": [0, 3, 2, 5, 2, ..],</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"bbox": [</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[236.98, 142.51, 24.7, 69.5],</t>
+  </si>
+  <si>
+    <t>[7.03, 167.76, 149.32, 94.87],</t>
+  </si>
+  <si>
+    <t>[557.21, 209.19, 81.35, 78.73],</t>
+  </si>
+  <si>
+    <t>[358.98, 218.05, 56.0, 102.83],</t>
+  </si>
+  <si>
+    <t>[290.69, 218.0, 61.83, 98.48],</t>
+  </si>
+  <si>
+    <t>],</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>},</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"class_id": [4, 9, 3, 1],</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[412.8, 157.61, 53.05, 138.01],</t>
+  </si>
+  <si>
+    <t>[384.43, 172.21, 15.12, 35.74],</t>
+  </si>
+  <si>
+    <t>[512.22, 205.75, 14.74, 15.97],</t>
+  </si>
+  <si>
+    <t>[493.1, 174.34, 20.29, 108.31],</t>
   </si>
 </sst>
 </file>
@@ -2634,13 +2697,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>207065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>231913</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2693,13 +2756,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>107676</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>198782</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2742,13 +2805,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>207065</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>140804</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>66261</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2791,13 +2854,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>198782</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>223631</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2850,13 +2913,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>118</xdr:row>
       <xdr:rowOff>124240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>182217</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>91109</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2902,13 +2965,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>91109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>124239</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2954,13 +3017,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>132520</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>215348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3013,13 +3076,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>165652</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3065,13 +3128,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>149087</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>107673</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>107674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3111,6 +3174,681 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>132520</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>207065</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>207064</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>231913</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="円/楕円 44"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2294281" y="17020761"/>
+          <a:ext cx="795131" cy="265043"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>207064</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>107675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>198782</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>99392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="直線矢印コネクタ 46"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3089412" y="16440979"/>
+          <a:ext cx="4075044" cy="712304"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>207064</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>198783</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直線矢印コネクタ 51"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="45" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3089412" y="20996413"/>
+          <a:ext cx="4075045" cy="2849217"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>140805</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>149088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>8281</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>24850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="四角形吹き出し 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4704522" y="20805914"/>
+          <a:ext cx="2509629" cy="1316936"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 58045"/>
+            <a:gd name="adj2" fmla="val -33726"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>&lt;&lt; bbox format &gt;&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>   [x, y, width,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> height]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>      x : left top position (x axis)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>      y : left top position (y axis)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>      width : width of bounding box</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>      height : height of bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>196550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>16564</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>143040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="四角形吹き出し 52"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="21093572"/>
+          <a:ext cx="1929847" cy="186685"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -60839"/>
+            <a:gd name="adj2" fmla="val 50712"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>class_id[0]'s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>204833</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>16564</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>151322</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="四角形吹き出し 57"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="21582246"/>
+          <a:ext cx="1929847" cy="186685"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54830"/>
+            <a:gd name="adj2" fmla="val 24092"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>class_id[2]'s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>200692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>16564</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>147181</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="四角形吹き出し 58"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="21337909"/>
+          <a:ext cx="1929847" cy="186685"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -58693"/>
+            <a:gd name="adj2" fmla="val 28529"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>class_id[1]'s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>208974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>16564</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>155464</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="四角形吹き出し 59"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="21826583"/>
+          <a:ext cx="1929847" cy="186685"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -54830"/>
+            <a:gd name="adj2" fmla="val 24092"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>class_id[3]'s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>213116</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>16564</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>159605</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="四角形吹き出し 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="22070920"/>
+          <a:ext cx="1929847" cy="186685"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -58264"/>
+            <a:gd name="adj2" fmla="val 37402"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>class_id[4]'s</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t> bounding box</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3451,10 +4189,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AQ101"/>
+  <dimension ref="B2:AQ134"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AY85" sqref="AY85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4290,7 +5028,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -4336,7 +5074,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -4382,7 +5120,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -4409,7 +5147,7 @@
       <c r="AC38" s="10"/>
       <c r="AD38" s="10"/>
       <c r="AE38" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF38" s="10"/>
       <c r="AG38" s="10"/>
@@ -4615,7 +5353,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
       <c r="H43" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
@@ -4639,7 +5377,7 @@
       <c r="AC43" s="10"/>
       <c r="AD43" s="10"/>
       <c r="AE43" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AF43" s="10"/>
       <c r="AG43" s="10"/>
@@ -4799,7 +5537,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
       <c r="H47" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
@@ -5016,59 +5754,59 @@
     </row>
     <row r="53" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E53" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD53" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F54" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE54" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E55" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD55" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F56" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AE56" s="4" t="s">
-        <v>76</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E57" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F58" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E59" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F60" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G61" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5174,7 +5912,7 @@
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
@@ -5221,7 +5959,7 @@
       <c r="C68" s="9"/>
       <c r="D68" s="10"/>
       <c r="E68" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
@@ -5296,7 +6034,7 @@
       <c r="AC69" s="10"/>
       <c r="AD69" s="10"/>
       <c r="AE69" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="AF69" s="10"/>
       <c r="AG69" s="10"/>
@@ -5412,7 +6150,7 @@
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I72" s="10"/>
       <c r="J72" s="10"/>
@@ -5459,7 +6197,7 @@
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I73" s="10"/>
       <c r="J73" s="10"/>
@@ -5531,7 +6269,7 @@
       <c r="AC74" s="10"/>
       <c r="AD74" s="10"/>
       <c r="AE74" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="AF74" s="10"/>
       <c r="AG74" s="10"/>
@@ -5732,69 +6470,108 @@
     </row>
     <row r="80" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C80" s="5" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C81" s="4" t="s">
+      <c r="C81" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AB81" s="4" t="s">
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
         <v>21</v>
       </c>
+      <c r="AC81" s="7"/>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7"/>
+      <c r="AK81" s="7"/>
+      <c r="AL81" s="7"/>
+      <c r="AM81" s="7"/>
+      <c r="AN81" s="7"/>
+      <c r="AO81" s="7"/>
+      <c r="AP81" s="7"/>
+      <c r="AQ81" s="8"/>
     </row>
     <row r="82" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C82" s="6"/>
-      <c r="D82" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="I82" s="7"/>
-      <c r="J82" s="7"/>
-      <c r="K82" s="7"/>
-      <c r="L82" s="7"/>
-      <c r="M82" s="7"/>
-      <c r="N82" s="7"/>
-      <c r="O82" s="7"/>
-      <c r="P82" s="7"/>
-      <c r="Q82" s="7"/>
-      <c r="R82" s="7"/>
-      <c r="S82" s="7"/>
-      <c r="T82" s="7"/>
-      <c r="U82" s="7"/>
-      <c r="V82" s="7"/>
-      <c r="W82" s="7"/>
-      <c r="X82" s="7"/>
-      <c r="Y82" s="7"/>
-      <c r="Z82" s="7"/>
-      <c r="AA82" s="7"/>
-      <c r="AB82" s="7"/>
-      <c r="AC82" s="7" t="s">
+      <c r="C82" s="9"/>
+      <c r="D82" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="AD82" s="7"/>
-      <c r="AE82" s="7"/>
-      <c r="AF82" s="7"/>
-      <c r="AG82" s="7"/>
-      <c r="AH82" s="7"/>
-      <c r="AI82" s="7"/>
-      <c r="AJ82" s="7"/>
-      <c r="AK82" s="7"/>
-      <c r="AL82" s="7"/>
-      <c r="AM82" s="7"/>
-      <c r="AN82" s="7"/>
-      <c r="AO82" s="7"/>
-      <c r="AP82" s="7"/>
-      <c r="AQ82" s="8"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
+      <c r="L82" s="10"/>
+      <c r="M82" s="10"/>
+      <c r="N82" s="10"/>
+      <c r="O82" s="10"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="10"/>
+      <c r="R82" s="10"/>
+      <c r="S82" s="10"/>
+      <c r="T82" s="10"/>
+      <c r="U82" s="10"/>
+      <c r="V82" s="10"/>
+      <c r="W82" s="10"/>
+      <c r="X82" s="10"/>
+      <c r="Y82" s="10"/>
+      <c r="Z82" s="10"/>
+      <c r="AA82" s="10"/>
+      <c r="AB82" s="10"/>
+      <c r="AC82" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD82" s="10"/>
+      <c r="AE82" s="10"/>
+      <c r="AF82" s="10"/>
+      <c r="AG82" s="10"/>
+      <c r="AH82" s="10"/>
+      <c r="AI82" s="10"/>
+      <c r="AJ82" s="10"/>
+      <c r="AK82" s="10"/>
+      <c r="AL82" s="10"/>
+      <c r="AM82" s="10"/>
+      <c r="AN82" s="10"/>
+      <c r="AO82" s="10"/>
+      <c r="AP82" s="10"/>
+      <c r="AQ82" s="11"/>
     </row>
     <row r="83" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C83" s="9"/>
       <c r="D83" s="10"/>
       <c r="E83" s="10" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
@@ -5821,7 +6598,7 @@
       <c r="AB83" s="10"/>
       <c r="AC83" s="10"/>
       <c r="AD83" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AE83" s="10"/>
       <c r="AF83" s="10"/>
@@ -5841,7 +6618,7 @@
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
       <c r="E84" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
@@ -5916,7 +6693,7 @@
       <c r="AC85" s="10"/>
       <c r="AD85" s="10"/>
       <c r="AE85" s="10" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="AF85" s="10"/>
       <c r="AG85" s="10"/>
@@ -5936,7 +6713,7 @@
       <c r="D86" s="10"/>
       <c r="E86" s="10"/>
       <c r="F86" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G86" s="10"/>
       <c r="H86" s="10"/>
@@ -5963,7 +6740,7 @@
       <c r="AC86" s="10"/>
       <c r="AD86" s="10"/>
       <c r="AE86" s="10" t="s">
-        <v>53</v>
+        <v>202</v>
       </c>
       <c r="AF86" s="10"/>
       <c r="AG86" s="10"/>
@@ -5984,7 +6761,7 @@
       <c r="E87" s="10"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
@@ -6009,10 +6786,10 @@
       <c r="AB87" s="10"/>
       <c r="AC87" s="10"/>
       <c r="AD87" s="10"/>
-      <c r="AE87" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF87" s="10"/>
+      <c r="AE87" s="10"/>
+      <c r="AF87" s="10" t="s">
+        <v>203</v>
+      </c>
       <c r="AG87" s="10"/>
       <c r="AH87" s="10"/>
       <c r="AI87" s="10"/>
@@ -6032,7 +6809,7 @@
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
       <c r="H88" s="10" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="I88" s="10"/>
       <c r="J88" s="10"/>
@@ -6056,10 +6833,10 @@
       <c r="AB88" s="10"/>
       <c r="AC88" s="10"/>
       <c r="AD88" s="10"/>
-      <c r="AE88" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF88" s="10"/>
+      <c r="AE88" s="10"/>
+      <c r="AF88" s="10" t="s">
+        <v>204</v>
+      </c>
       <c r="AG88" s="10"/>
       <c r="AH88" s="10"/>
       <c r="AI88" s="10"/>
@@ -6079,7 +6856,7 @@
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
       <c r="H89" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="I89" s="10"/>
       <c r="J89" s="10"/>
@@ -6103,11 +6880,11 @@
       <c r="AB89" s="10"/>
       <c r="AC89" s="10"/>
       <c r="AD89" s="10"/>
-      <c r="AE89" s="10" t="s">
-        <v>55</v>
-      </c>
+      <c r="AE89" s="10"/>
       <c r="AF89" s="10"/>
-      <c r="AG89" s="10"/>
+      <c r="AG89" s="10" t="s">
+        <v>205</v>
+      </c>
       <c r="AH89" s="10"/>
       <c r="AI89" s="10"/>
       <c r="AJ89" s="10"/>
@@ -6125,7 +6902,7 @@
       <c r="E90" s="10"/>
       <c r="F90" s="10"/>
       <c r="G90" s="10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H90" s="10"/>
       <c r="I90" s="10"/>
@@ -6149,12 +6926,12 @@
       <c r="AA90" s="10"/>
       <c r="AB90" s="10"/>
       <c r="AC90" s="10"/>
-      <c r="AD90" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="AD90" s="10"/>
       <c r="AE90" s="10"/>
       <c r="AF90" s="10"/>
-      <c r="AG90" s="10"/>
+      <c r="AG90" s="10" t="s">
+        <v>206</v>
+      </c>
       <c r="AH90" s="10"/>
       <c r="AI90" s="10"/>
       <c r="AJ90" s="10"/>
@@ -6170,10 +6947,10 @@
       <c r="C91" s="9"/>
       <c r="D91" s="10"/>
       <c r="E91" s="10"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="F91" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G91" s="10"/>
       <c r="H91" s="10"/>
       <c r="I91" s="10"/>
       <c r="J91" s="10"/>
@@ -6196,12 +6973,12 @@
       <c r="AA91" s="10"/>
       <c r="AB91" s="10"/>
       <c r="AC91" s="10"/>
-      <c r="AD91" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="AD91" s="10"/>
       <c r="AE91" s="10"/>
       <c r="AF91" s="10"/>
-      <c r="AG91" s="10"/>
+      <c r="AG91" s="10" t="s">
+        <v>207</v>
+      </c>
       <c r="AH91" s="10"/>
       <c r="AI91" s="10"/>
       <c r="AJ91" s="10"/>
@@ -6215,13 +6992,13 @@
     </row>
     <row r="92" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C92" s="9"/>
-      <c r="D92" s="10"/>
+      <c r="D92" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="E92" s="10"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
-      <c r="H92" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="H92" s="10"/>
       <c r="I92" s="10"/>
       <c r="J92" s="10"/>
       <c r="K92" s="10"/>
@@ -6244,11 +7021,11 @@
       <c r="AB92" s="10"/>
       <c r="AC92" s="10"/>
       <c r="AD92" s="10"/>
-      <c r="AE92" s="10" t="s">
-        <v>31</v>
-      </c>
+      <c r="AE92" s="10"/>
       <c r="AF92" s="10"/>
-      <c r="AG92" s="10"/>
+      <c r="AG92" s="10" t="s">
+        <v>208</v>
+      </c>
       <c r="AH92" s="10"/>
       <c r="AI92" s="10"/>
       <c r="AJ92" s="10"/>
@@ -6266,9 +7043,7 @@
       <c r="E93" s="10"/>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
-      <c r="H93" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="H93" s="10"/>
       <c r="I93" s="10"/>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
@@ -6291,11 +7066,11 @@
       <c r="AB93" s="10"/>
       <c r="AC93" s="10"/>
       <c r="AD93" s="10"/>
-      <c r="AE93" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="AE93" s="10"/>
       <c r="AF93" s="10"/>
-      <c r="AG93" s="10"/>
+      <c r="AG93" s="10" t="s">
+        <v>209</v>
+      </c>
       <c r="AH93" s="10"/>
       <c r="AI93" s="10"/>
       <c r="AJ93" s="10"/>
@@ -6312,9 +7087,7 @@
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
       <c r="F94" s="10"/>
-      <c r="G94" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="G94" s="10"/>
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
       <c r="J94" s="10"/>
@@ -6338,11 +7111,11 @@
       <c r="AB94" s="10"/>
       <c r="AC94" s="10"/>
       <c r="AD94" s="10"/>
-      <c r="AE94" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="AE94" s="10"/>
       <c r="AF94" s="10"/>
-      <c r="AG94" s="10"/>
+      <c r="AG94" s="10" t="s">
+        <v>211</v>
+      </c>
       <c r="AH94" s="10"/>
       <c r="AI94" s="10"/>
       <c r="AJ94" s="10"/>
@@ -6359,9 +7132,7 @@
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
-      <c r="G95" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="G95" s="10"/>
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
       <c r="J95" s="10"/>
@@ -6385,10 +7156,10 @@
       <c r="AB95" s="10"/>
       <c r="AC95" s="10"/>
       <c r="AD95" s="10"/>
-      <c r="AE95" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF95" s="10"/>
+      <c r="AE95" s="10"/>
+      <c r="AF95" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="AG95" s="10"/>
       <c r="AH95" s="10"/>
       <c r="AI95" s="10"/>
@@ -6407,9 +7178,7 @@
       <c r="E96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
-      <c r="H96" s="10" t="s">
-        <v>50</v>
-      </c>
+      <c r="H96" s="10"/>
       <c r="I96" s="10"/>
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
@@ -6433,7 +7202,7 @@
       <c r="AC96" s="10"/>
       <c r="AD96" s="10"/>
       <c r="AE96" s="10" t="s">
-        <v>56</v>
+        <v>212</v>
       </c>
       <c r="AF96" s="10"/>
       <c r="AG96" s="10"/>
@@ -6454,9 +7223,7 @@
       <c r="E97" s="10"/>
       <c r="F97" s="10"/>
       <c r="G97" s="10"/>
-      <c r="H97" s="10" t="s">
-        <v>48</v>
-      </c>
+      <c r="H97" s="10"/>
       <c r="I97" s="10"/>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
@@ -6478,10 +7245,10 @@
       <c r="AA97" s="10"/>
       <c r="AB97" s="10"/>
       <c r="AC97" s="10"/>
-      <c r="AD97" s="10"/>
-      <c r="AE97" s="10" t="s">
-        <v>60</v>
-      </c>
+      <c r="AD97" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE97" s="10"/>
       <c r="AF97" s="10"/>
       <c r="AG97" s="10"/>
       <c r="AH97" s="10"/>
@@ -6500,9 +7267,7 @@
       <c r="D98" s="10"/>
       <c r="E98" s="10"/>
       <c r="F98" s="10"/>
-      <c r="G98" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="G98" s="10"/>
       <c r="H98" s="10"/>
       <c r="I98" s="10"/>
       <c r="J98" s="10"/>
@@ -6526,7 +7291,7 @@
       <c r="AB98" s="10"/>
       <c r="AC98" s="10"/>
       <c r="AD98" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="AE98" s="10"/>
       <c r="AF98" s="10"/>
@@ -6547,9 +7312,7 @@
       <c r="D99" s="10"/>
       <c r="E99" s="10"/>
       <c r="F99" s="10"/>
-      <c r="G99" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="G99" s="10"/>
       <c r="H99" s="10"/>
       <c r="I99" s="10"/>
       <c r="J99" s="10"/>
@@ -6571,11 +7334,11 @@
       <c r="Z99" s="10"/>
       <c r="AA99" s="10"/>
       <c r="AB99" s="10"/>
-      <c r="AC99" s="10" t="s">
-        <v>25</v>
-      </c>
+      <c r="AC99" s="10"/>
       <c r="AD99" s="10"/>
-      <c r="AE99" s="10"/>
+      <c r="AE99" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="AF99" s="10"/>
       <c r="AG99" s="10"/>
       <c r="AH99" s="10"/>
@@ -6593,9 +7356,7 @@
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
       <c r="E100" s="10"/>
-      <c r="F100" s="10" t="s">
-        <v>26</v>
-      </c>
+      <c r="F100" s="10"/>
       <c r="G100" s="10"/>
       <c r="H100" s="10"/>
       <c r="I100" s="10"/>
@@ -6620,7 +7381,9 @@
       <c r="AB100" s="10"/>
       <c r="AC100" s="10"/>
       <c r="AD100" s="10"/>
-      <c r="AE100" s="10"/>
+      <c r="AE100" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="AF100" s="10"/>
       <c r="AG100" s="10"/>
       <c r="AH100" s="10"/>
@@ -6635,49 +7398,1491 @@
       <c r="AQ100" s="11"/>
     </row>
     <row r="101" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C101" s="12"/>
-      <c r="D101" s="13" t="s">
+      <c r="C101" s="9"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10"/>
+      <c r="K101" s="10"/>
+      <c r="L101" s="10"/>
+      <c r="M101" s="10"/>
+      <c r="N101" s="10"/>
+      <c r="O101" s="10"/>
+      <c r="P101" s="10"/>
+      <c r="Q101" s="10"/>
+      <c r="R101" s="10"/>
+      <c r="S101" s="10"/>
+      <c r="T101" s="10"/>
+      <c r="U101" s="10"/>
+      <c r="V101" s="10"/>
+      <c r="W101" s="10"/>
+      <c r="X101" s="10"/>
+      <c r="Y101" s="10"/>
+      <c r="Z101" s="10"/>
+      <c r="AA101" s="10"/>
+      <c r="AB101" s="10"/>
+      <c r="AC101" s="10"/>
+      <c r="AD101" s="10"/>
+      <c r="AE101" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="AF101" s="10"/>
+      <c r="AG101" s="10"/>
+      <c r="AH101" s="10"/>
+      <c r="AI101" s="10"/>
+      <c r="AJ101" s="10"/>
+      <c r="AK101" s="10"/>
+      <c r="AL101" s="10"/>
+      <c r="AM101" s="10"/>
+      <c r="AN101" s="10"/>
+      <c r="AO101" s="10"/>
+      <c r="AP101" s="10"/>
+      <c r="AQ101" s="11"/>
+    </row>
+    <row r="102" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C102" s="9"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+      <c r="J102" s="10"/>
+      <c r="K102" s="10"/>
+      <c r="L102" s="10"/>
+      <c r="M102" s="10"/>
+      <c r="N102" s="10"/>
+      <c r="O102" s="10"/>
+      <c r="P102" s="10"/>
+      <c r="Q102" s="10"/>
+      <c r="R102" s="10"/>
+      <c r="S102" s="10"/>
+      <c r="T102" s="10"/>
+      <c r="U102" s="10"/>
+      <c r="V102" s="10"/>
+      <c r="W102" s="10"/>
+      <c r="X102" s="10"/>
+      <c r="Y102" s="10"/>
+      <c r="Z102" s="10"/>
+      <c r="AA102" s="10"/>
+      <c r="AB102" s="10"/>
+      <c r="AC102" s="10"/>
+      <c r="AD102" s="10"/>
+      <c r="AE102" s="10"/>
+      <c r="AF102" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG102" s="10"/>
+      <c r="AH102" s="10"/>
+      <c r="AI102" s="10"/>
+      <c r="AJ102" s="10"/>
+      <c r="AK102" s="10"/>
+      <c r="AL102" s="10"/>
+      <c r="AM102" s="10"/>
+      <c r="AN102" s="10"/>
+      <c r="AO102" s="10"/>
+      <c r="AP102" s="10"/>
+      <c r="AQ102" s="11"/>
+    </row>
+    <row r="103" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C103" s="9"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
+      <c r="M103" s="10"/>
+      <c r="N103" s="10"/>
+      <c r="O103" s="10"/>
+      <c r="P103" s="10"/>
+      <c r="Q103" s="10"/>
+      <c r="R103" s="10"/>
+      <c r="S103" s="10"/>
+      <c r="T103" s="10"/>
+      <c r="U103" s="10"/>
+      <c r="V103" s="10"/>
+      <c r="W103" s="10"/>
+      <c r="X103" s="10"/>
+      <c r="Y103" s="10"/>
+      <c r="Z103" s="10"/>
+      <c r="AA103" s="10"/>
+      <c r="AB103" s="10"/>
+      <c r="AC103" s="10"/>
+      <c r="AD103" s="10"/>
+      <c r="AE103" s="10"/>
+      <c r="AF103" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG103" s="10"/>
+      <c r="AH103" s="10"/>
+      <c r="AI103" s="10"/>
+      <c r="AJ103" s="10"/>
+      <c r="AK103" s="10"/>
+      <c r="AL103" s="10"/>
+      <c r="AM103" s="10"/>
+      <c r="AN103" s="10"/>
+      <c r="AO103" s="10"/>
+      <c r="AP103" s="10"/>
+      <c r="AQ103" s="11"/>
+    </row>
+    <row r="104" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C104" s="9"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10"/>
+      <c r="K104" s="10"/>
+      <c r="L104" s="10"/>
+      <c r="M104" s="10"/>
+      <c r="N104" s="10"/>
+      <c r="O104" s="10"/>
+      <c r="P104" s="10"/>
+      <c r="Q104" s="10"/>
+      <c r="R104" s="10"/>
+      <c r="S104" s="10"/>
+      <c r="T104" s="10"/>
+      <c r="U104" s="10"/>
+      <c r="V104" s="10"/>
+      <c r="W104" s="10"/>
+      <c r="X104" s="10"/>
+      <c r="Y104" s="10"/>
+      <c r="Z104" s="10"/>
+      <c r="AA104" s="10"/>
+      <c r="AB104" s="10"/>
+      <c r="AC104" s="10"/>
+      <c r="AD104" s="10"/>
+      <c r="AE104" s="10"/>
+      <c r="AF104" s="10"/>
+      <c r="AG104" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH104" s="10"/>
+      <c r="AI104" s="10"/>
+      <c r="AJ104" s="10"/>
+      <c r="AK104" s="10"/>
+      <c r="AL104" s="10"/>
+      <c r="AM104" s="10"/>
+      <c r="AN104" s="10"/>
+      <c r="AO104" s="10"/>
+      <c r="AP104" s="10"/>
+      <c r="AQ104" s="11"/>
+    </row>
+    <row r="105" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C105" s="9"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
+      <c r="K105" s="10"/>
+      <c r="L105" s="10"/>
+      <c r="M105" s="10"/>
+      <c r="N105" s="10"/>
+      <c r="O105" s="10"/>
+      <c r="P105" s="10"/>
+      <c r="Q105" s="10"/>
+      <c r="R105" s="10"/>
+      <c r="S105" s="10"/>
+      <c r="T105" s="10"/>
+      <c r="U105" s="10"/>
+      <c r="V105" s="10"/>
+      <c r="W105" s="10"/>
+      <c r="X105" s="10"/>
+      <c r="Y105" s="10"/>
+      <c r="Z105" s="10"/>
+      <c r="AA105" s="10"/>
+      <c r="AB105" s="10"/>
+      <c r="AC105" s="10"/>
+      <c r="AD105" s="10"/>
+      <c r="AE105" s="10"/>
+      <c r="AF105" s="10"/>
+      <c r="AG105" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="AH105" s="10"/>
+      <c r="AI105" s="10"/>
+      <c r="AJ105" s="10"/>
+      <c r="AK105" s="10"/>
+      <c r="AL105" s="10"/>
+      <c r="AM105" s="10"/>
+      <c r="AN105" s="10"/>
+      <c r="AO105" s="10"/>
+      <c r="AP105" s="10"/>
+      <c r="AQ105" s="11"/>
+    </row>
+    <row r="106" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C106" s="9"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
+      <c r="K106" s="10"/>
+      <c r="L106" s="10"/>
+      <c r="M106" s="10"/>
+      <c r="N106" s="10"/>
+      <c r="O106" s="10"/>
+      <c r="P106" s="10"/>
+      <c r="Q106" s="10"/>
+      <c r="R106" s="10"/>
+      <c r="S106" s="10"/>
+      <c r="T106" s="10"/>
+      <c r="U106" s="10"/>
+      <c r="V106" s="10"/>
+      <c r="W106" s="10"/>
+      <c r="X106" s="10"/>
+      <c r="Y106" s="10"/>
+      <c r="Z106" s="10"/>
+      <c r="AA106" s="10"/>
+      <c r="AB106" s="10"/>
+      <c r="AC106" s="10"/>
+      <c r="AD106" s="10"/>
+      <c r="AE106" s="10"/>
+      <c r="AF106" s="10"/>
+      <c r="AG106" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="AH106" s="10"/>
+      <c r="AI106" s="10"/>
+      <c r="AJ106" s="10"/>
+      <c r="AK106" s="10"/>
+      <c r="AL106" s="10"/>
+      <c r="AM106" s="10"/>
+      <c r="AN106" s="10"/>
+      <c r="AO106" s="10"/>
+      <c r="AP106" s="10"/>
+      <c r="AQ106" s="11"/>
+    </row>
+    <row r="107" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C107" s="9"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
+      <c r="L107" s="10"/>
+      <c r="M107" s="10"/>
+      <c r="N107" s="10"/>
+      <c r="O107" s="10"/>
+      <c r="P107" s="10"/>
+      <c r="Q107" s="10"/>
+      <c r="R107" s="10"/>
+      <c r="S107" s="10"/>
+      <c r="T107" s="10"/>
+      <c r="U107" s="10"/>
+      <c r="V107" s="10"/>
+      <c r="W107" s="10"/>
+      <c r="X107" s="10"/>
+      <c r="Y107" s="10"/>
+      <c r="Z107" s="10"/>
+      <c r="AA107" s="10"/>
+      <c r="AB107" s="10"/>
+      <c r="AC107" s="10"/>
+      <c r="AD107" s="10"/>
+      <c r="AE107" s="10"/>
+      <c r="AF107" s="10"/>
+      <c r="AG107" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH107" s="10"/>
+      <c r="AI107" s="10"/>
+      <c r="AJ107" s="10"/>
+      <c r="AK107" s="10"/>
+      <c r="AL107" s="10"/>
+      <c r="AM107" s="10"/>
+      <c r="AN107" s="10"/>
+      <c r="AO107" s="10"/>
+      <c r="AP107" s="10"/>
+      <c r="AQ107" s="11"/>
+    </row>
+    <row r="108" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C108" s="9"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
+      <c r="H108" s="10"/>
+      <c r="I108" s="10"/>
+      <c r="J108" s="10"/>
+      <c r="K108" s="10"/>
+      <c r="L108" s="10"/>
+      <c r="M108" s="10"/>
+      <c r="N108" s="10"/>
+      <c r="O108" s="10"/>
+      <c r="P108" s="10"/>
+      <c r="Q108" s="10"/>
+      <c r="R108" s="10"/>
+      <c r="S108" s="10"/>
+      <c r="T108" s="10"/>
+      <c r="U108" s="10"/>
+      <c r="V108" s="10"/>
+      <c r="W108" s="10"/>
+      <c r="X108" s="10"/>
+      <c r="Y108" s="10"/>
+      <c r="Z108" s="10"/>
+      <c r="AA108" s="10"/>
+      <c r="AB108" s="10"/>
+      <c r="AC108" s="10"/>
+      <c r="AD108" s="10"/>
+      <c r="AE108" s="10"/>
+      <c r="AF108" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG108" s="10"/>
+      <c r="AH108" s="10"/>
+      <c r="AI108" s="10"/>
+      <c r="AJ108" s="10"/>
+      <c r="AK108" s="10"/>
+      <c r="AL108" s="10"/>
+      <c r="AM108" s="10"/>
+      <c r="AN108" s="10"/>
+      <c r="AO108" s="10"/>
+      <c r="AP108" s="10"/>
+      <c r="AQ108" s="11"/>
+    </row>
+    <row r="109" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C109" s="9"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
+      <c r="H109" s="10"/>
+      <c r="I109" s="10"/>
+      <c r="J109" s="10"/>
+      <c r="K109" s="10"/>
+      <c r="L109" s="10"/>
+      <c r="M109" s="10"/>
+      <c r="N109" s="10"/>
+      <c r="O109" s="10"/>
+      <c r="P109" s="10"/>
+      <c r="Q109" s="10"/>
+      <c r="R109" s="10"/>
+      <c r="S109" s="10"/>
+      <c r="T109" s="10"/>
+      <c r="U109" s="10"/>
+      <c r="V109" s="10"/>
+      <c r="W109" s="10"/>
+      <c r="X109" s="10"/>
+      <c r="Y109" s="10"/>
+      <c r="Z109" s="10"/>
+      <c r="AA109" s="10"/>
+      <c r="AB109" s="10"/>
+      <c r="AC109" s="10"/>
+      <c r="AD109" s="10"/>
+      <c r="AE109" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF109" s="10"/>
+      <c r="AG109" s="10"/>
+      <c r="AH109" s="10"/>
+      <c r="AI109" s="10"/>
+      <c r="AJ109" s="10"/>
+      <c r="AK109" s="10"/>
+      <c r="AL109" s="10"/>
+      <c r="AM109" s="10"/>
+      <c r="AN109" s="10"/>
+      <c r="AO109" s="10"/>
+      <c r="AP109" s="10"/>
+      <c r="AQ109" s="11"/>
+    </row>
+    <row r="110" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C110" s="9"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
+      <c r="H110" s="10"/>
+      <c r="I110" s="10"/>
+      <c r="J110" s="10"/>
+      <c r="K110" s="10"/>
+      <c r="L110" s="10"/>
+      <c r="M110" s="10"/>
+      <c r="N110" s="10"/>
+      <c r="O110" s="10"/>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="10"/>
+      <c r="R110" s="10"/>
+      <c r="S110" s="10"/>
+      <c r="T110" s="10"/>
+      <c r="U110" s="10"/>
+      <c r="V110" s="10"/>
+      <c r="W110" s="10"/>
+      <c r="X110" s="10"/>
+      <c r="Y110" s="10"/>
+      <c r="Z110" s="10"/>
+      <c r="AA110" s="10"/>
+      <c r="AB110" s="10"/>
+      <c r="AC110" s="10"/>
+      <c r="AD110" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="AE110" s="10"/>
+      <c r="AF110" s="10"/>
+      <c r="AG110" s="10"/>
+      <c r="AH110" s="10"/>
+      <c r="AI110" s="10"/>
+      <c r="AJ110" s="10"/>
+      <c r="AK110" s="10"/>
+      <c r="AL110" s="10"/>
+      <c r="AM110" s="10"/>
+      <c r="AN110" s="10"/>
+      <c r="AO110" s="10"/>
+      <c r="AP110" s="10"/>
+      <c r="AQ110" s="11"/>
+    </row>
+    <row r="111" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C111" s="12"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
+      <c r="M111" s="13"/>
+      <c r="N111" s="13"/>
+      <c r="O111" s="13"/>
+      <c r="P111" s="13"/>
+      <c r="Q111" s="13"/>
+      <c r="R111" s="13"/>
+      <c r="S111" s="13"/>
+      <c r="T111" s="13"/>
+      <c r="U111" s="13"/>
+      <c r="V111" s="13"/>
+      <c r="W111" s="13"/>
+      <c r="X111" s="13"/>
+      <c r="Y111" s="13"/>
+      <c r="Z111" s="13"/>
+      <c r="AA111" s="13"/>
+      <c r="AB111" s="13"/>
+      <c r="AC111" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="13"/>
-      <c r="N101" s="13"/>
-      <c r="O101" s="13"/>
-      <c r="P101" s="13"/>
-      <c r="Q101" s="13"/>
-      <c r="R101" s="13"/>
-      <c r="S101" s="13"/>
-      <c r="T101" s="13"/>
-      <c r="U101" s="13"/>
-      <c r="V101" s="13"/>
-      <c r="W101" s="13"/>
-      <c r="X101" s="13"/>
-      <c r="Y101" s="13"/>
-      <c r="Z101" s="13"/>
-      <c r="AA101" s="13"/>
-      <c r="AB101" s="13"/>
-      <c r="AC101" s="13"/>
-      <c r="AD101" s="13"/>
-      <c r="AE101" s="13"/>
-      <c r="AF101" s="13"/>
-      <c r="AG101" s="13"/>
-      <c r="AH101" s="13"/>
-      <c r="AI101" s="13"/>
-      <c r="AJ101" s="13"/>
-      <c r="AK101" s="13"/>
-      <c r="AL101" s="13"/>
-      <c r="AM101" s="13"/>
-      <c r="AN101" s="13"/>
-      <c r="AO101" s="13"/>
-      <c r="AP101" s="13"/>
-      <c r="AQ101" s="14"/>
+      <c r="AD111" s="13"/>
+      <c r="AE111" s="13"/>
+      <c r="AF111" s="13"/>
+      <c r="AG111" s="13"/>
+      <c r="AH111" s="13"/>
+      <c r="AI111" s="13"/>
+      <c r="AJ111" s="13"/>
+      <c r="AK111" s="13"/>
+      <c r="AL111" s="13"/>
+      <c r="AM111" s="13"/>
+      <c r="AN111" s="13"/>
+      <c r="AO111" s="13"/>
+      <c r="AP111" s="13"/>
+      <c r="AQ111" s="14"/>
+    </row>
+    <row r="112" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
+      <c r="H112" s="10"/>
+      <c r="I112" s="10"/>
+      <c r="J112" s="10"/>
+      <c r="K112" s="10"/>
+      <c r="L112" s="10"/>
+      <c r="M112" s="10"/>
+      <c r="N112" s="10"/>
+      <c r="O112" s="10"/>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="10"/>
+      <c r="R112" s="10"/>
+      <c r="S112" s="10"/>
+      <c r="T112" s="10"/>
+      <c r="U112" s="10"/>
+      <c r="V112" s="10"/>
+      <c r="W112" s="10"/>
+      <c r="X112" s="10"/>
+      <c r="Y112" s="10"/>
+      <c r="Z112" s="10"/>
+      <c r="AA112" s="10"/>
+      <c r="AB112" s="10"/>
+      <c r="AC112" s="10"/>
+      <c r="AD112" s="10"/>
+      <c r="AE112" s="10"/>
+      <c r="AF112" s="10"/>
+      <c r="AG112" s="10"/>
+      <c r="AH112" s="10"/>
+      <c r="AI112" s="10"/>
+      <c r="AJ112" s="10"/>
+      <c r="AK112" s="10"/>
+      <c r="AL112" s="10"/>
+      <c r="AM112" s="10"/>
+      <c r="AN112" s="10"/>
+      <c r="AO112" s="10"/>
+      <c r="AP112" s="10"/>
+      <c r="AQ112" s="10"/>
+    </row>
+    <row r="113" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C113" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="114" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C114" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB114" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C115" s="6"/>
+      <c r="D115" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="7"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="7"/>
+      <c r="P115" s="7"/>
+      <c r="Q115" s="7"/>
+      <c r="R115" s="7"/>
+      <c r="S115" s="7"/>
+      <c r="T115" s="7"/>
+      <c r="U115" s="7"/>
+      <c r="V115" s="7"/>
+      <c r="W115" s="7"/>
+      <c r="X115" s="7"/>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7"/>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7"/>
+      <c r="AC115" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD115" s="7"/>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7"/>
+      <c r="AL115" s="7"/>
+      <c r="AM115" s="7"/>
+      <c r="AN115" s="7"/>
+      <c r="AO115" s="7"/>
+      <c r="AP115" s="7"/>
+      <c r="AQ115" s="8"/>
+    </row>
+    <row r="116" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C116" s="9"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" s="10"/>
+      <c r="G116" s="10"/>
+      <c r="H116" s="10"/>
+      <c r="I116" s="10"/>
+      <c r="J116" s="10"/>
+      <c r="K116" s="10"/>
+      <c r="L116" s="10"/>
+      <c r="M116" s="10"/>
+      <c r="N116" s="10"/>
+      <c r="O116" s="10"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="10"/>
+      <c r="R116" s="10"/>
+      <c r="S116" s="10"/>
+      <c r="T116" s="10"/>
+      <c r="U116" s="10"/>
+      <c r="V116" s="10"/>
+      <c r="W116" s="10"/>
+      <c r="X116" s="10"/>
+      <c r="Y116" s="10"/>
+      <c r="Z116" s="10"/>
+      <c r="AA116" s="10"/>
+      <c r="AB116" s="10"/>
+      <c r="AC116" s="10"/>
+      <c r="AD116" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE116" s="10"/>
+      <c r="AF116" s="10"/>
+      <c r="AG116" s="10"/>
+      <c r="AH116" s="10"/>
+      <c r="AI116" s="10"/>
+      <c r="AJ116" s="10"/>
+      <c r="AK116" s="10"/>
+      <c r="AL116" s="10"/>
+      <c r="AM116" s="10"/>
+      <c r="AN116" s="10"/>
+      <c r="AO116" s="10"/>
+      <c r="AP116" s="10"/>
+      <c r="AQ116" s="11"/>
+    </row>
+    <row r="117" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C117" s="9"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="10"/>
+      <c r="J117" s="10"/>
+      <c r="K117" s="10"/>
+      <c r="L117" s="10"/>
+      <c r="M117" s="10"/>
+      <c r="N117" s="10"/>
+      <c r="O117" s="10"/>
+      <c r="P117" s="10"/>
+      <c r="Q117" s="10"/>
+      <c r="R117" s="10"/>
+      <c r="S117" s="10"/>
+      <c r="T117" s="10"/>
+      <c r="U117" s="10"/>
+      <c r="V117" s="10"/>
+      <c r="W117" s="10"/>
+      <c r="X117" s="10"/>
+      <c r="Y117" s="10"/>
+      <c r="Z117" s="10"/>
+      <c r="AA117" s="10"/>
+      <c r="AB117" s="10"/>
+      <c r="AC117" s="10"/>
+      <c r="AD117" s="10"/>
+      <c r="AE117" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF117" s="10"/>
+      <c r="AG117" s="10"/>
+      <c r="AH117" s="10"/>
+      <c r="AI117" s="10"/>
+      <c r="AJ117" s="10"/>
+      <c r="AK117" s="10"/>
+      <c r="AL117" s="10"/>
+      <c r="AM117" s="10"/>
+      <c r="AN117" s="10"/>
+      <c r="AO117" s="10"/>
+      <c r="AP117" s="10"/>
+      <c r="AQ117" s="11"/>
+    </row>
+    <row r="118" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C118" s="9"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
+      <c r="H118" s="10"/>
+      <c r="I118" s="10"/>
+      <c r="J118" s="10"/>
+      <c r="K118" s="10"/>
+      <c r="L118" s="10"/>
+      <c r="M118" s="10"/>
+      <c r="N118" s="10"/>
+      <c r="O118" s="10"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="10"/>
+      <c r="R118" s="10"/>
+      <c r="S118" s="10"/>
+      <c r="T118" s="10"/>
+      <c r="U118" s="10"/>
+      <c r="V118" s="10"/>
+      <c r="W118" s="10"/>
+      <c r="X118" s="10"/>
+      <c r="Y118" s="10"/>
+      <c r="Z118" s="10"/>
+      <c r="AA118" s="10"/>
+      <c r="AB118" s="10"/>
+      <c r="AC118" s="10"/>
+      <c r="AD118" s="10"/>
+      <c r="AE118" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF118" s="10"/>
+      <c r="AG118" s="10"/>
+      <c r="AH118" s="10"/>
+      <c r="AI118" s="10"/>
+      <c r="AJ118" s="10"/>
+      <c r="AK118" s="10"/>
+      <c r="AL118" s="10"/>
+      <c r="AM118" s="10"/>
+      <c r="AN118" s="10"/>
+      <c r="AO118" s="10"/>
+      <c r="AP118" s="10"/>
+      <c r="AQ118" s="11"/>
+    </row>
+    <row r="119" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C119" s="9"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G119" s="10"/>
+      <c r="H119" s="10"/>
+      <c r="I119" s="10"/>
+      <c r="J119" s="10"/>
+      <c r="K119" s="10"/>
+      <c r="L119" s="10"/>
+      <c r="M119" s="10"/>
+      <c r="N119" s="10"/>
+      <c r="O119" s="10"/>
+      <c r="P119" s="10"/>
+      <c r="Q119" s="10"/>
+      <c r="R119" s="10"/>
+      <c r="S119" s="10"/>
+      <c r="T119" s="10"/>
+      <c r="U119" s="10"/>
+      <c r="V119" s="10"/>
+      <c r="W119" s="10"/>
+      <c r="X119" s="10"/>
+      <c r="Y119" s="10"/>
+      <c r="Z119" s="10"/>
+      <c r="AA119" s="10"/>
+      <c r="AB119" s="10"/>
+      <c r="AC119" s="10"/>
+      <c r="AD119" s="10"/>
+      <c r="AE119" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF119" s="10"/>
+      <c r="AG119" s="10"/>
+      <c r="AH119" s="10"/>
+      <c r="AI119" s="10"/>
+      <c r="AJ119" s="10"/>
+      <c r="AK119" s="10"/>
+      <c r="AL119" s="10"/>
+      <c r="AM119" s="10"/>
+      <c r="AN119" s="10"/>
+      <c r="AO119" s="10"/>
+      <c r="AP119" s="10"/>
+      <c r="AQ119" s="11"/>
+    </row>
+    <row r="120" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C120" s="9"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H120" s="10"/>
+      <c r="I120" s="10"/>
+      <c r="J120" s="10"/>
+      <c r="K120" s="10"/>
+      <c r="L120" s="10"/>
+      <c r="M120" s="10"/>
+      <c r="N120" s="10"/>
+      <c r="O120" s="10"/>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="10"/>
+      <c r="R120" s="10"/>
+      <c r="S120" s="10"/>
+      <c r="T120" s="10"/>
+      <c r="U120" s="10"/>
+      <c r="V120" s="10"/>
+      <c r="W120" s="10"/>
+      <c r="X120" s="10"/>
+      <c r="Y120" s="10"/>
+      <c r="Z120" s="10"/>
+      <c r="AA120" s="10"/>
+      <c r="AB120" s="10"/>
+      <c r="AC120" s="10"/>
+      <c r="AD120" s="10"/>
+      <c r="AE120" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF120" s="10"/>
+      <c r="AG120" s="10"/>
+      <c r="AH120" s="10"/>
+      <c r="AI120" s="10"/>
+      <c r="AJ120" s="10"/>
+      <c r="AK120" s="10"/>
+      <c r="AL120" s="10"/>
+      <c r="AM120" s="10"/>
+      <c r="AN120" s="10"/>
+      <c r="AO120" s="10"/>
+      <c r="AP120" s="10"/>
+      <c r="AQ120" s="11"/>
+    </row>
+    <row r="121" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C121" s="9"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
+      <c r="H121" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I121" s="10"/>
+      <c r="J121" s="10"/>
+      <c r="K121" s="10"/>
+      <c r="L121" s="10"/>
+      <c r="M121" s="10"/>
+      <c r="N121" s="10"/>
+      <c r="O121" s="10"/>
+      <c r="P121" s="10"/>
+      <c r="Q121" s="10"/>
+      <c r="R121" s="10"/>
+      <c r="S121" s="10"/>
+      <c r="T121" s="10"/>
+      <c r="U121" s="10"/>
+      <c r="V121" s="10"/>
+      <c r="W121" s="10"/>
+      <c r="X121" s="10"/>
+      <c r="Y121" s="10"/>
+      <c r="Z121" s="10"/>
+      <c r="AA121" s="10"/>
+      <c r="AB121" s="10"/>
+      <c r="AC121" s="10"/>
+      <c r="AD121" s="10"/>
+      <c r="AE121" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF121" s="10"/>
+      <c r="AG121" s="10"/>
+      <c r="AH121" s="10"/>
+      <c r="AI121" s="10"/>
+      <c r="AJ121" s="10"/>
+      <c r="AK121" s="10"/>
+      <c r="AL121" s="10"/>
+      <c r="AM121" s="10"/>
+      <c r="AN121" s="10"/>
+      <c r="AO121" s="10"/>
+      <c r="AP121" s="10"/>
+      <c r="AQ121" s="11"/>
+    </row>
+    <row r="122" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C122" s="9"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
+      <c r="H122" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I122" s="10"/>
+      <c r="J122" s="10"/>
+      <c r="K122" s="10"/>
+      <c r="L122" s="10"/>
+      <c r="M122" s="10"/>
+      <c r="N122" s="10"/>
+      <c r="O122" s="10"/>
+      <c r="P122" s="10"/>
+      <c r="Q122" s="10"/>
+      <c r="R122" s="10"/>
+      <c r="S122" s="10"/>
+      <c r="T122" s="10"/>
+      <c r="U122" s="10"/>
+      <c r="V122" s="10"/>
+      <c r="W122" s="10"/>
+      <c r="X122" s="10"/>
+      <c r="Y122" s="10"/>
+      <c r="Z122" s="10"/>
+      <c r="AA122" s="10"/>
+      <c r="AB122" s="10"/>
+      <c r="AC122" s="10"/>
+      <c r="AD122" s="10"/>
+      <c r="AE122" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF122" s="10"/>
+      <c r="AG122" s="10"/>
+      <c r="AH122" s="10"/>
+      <c r="AI122" s="10"/>
+      <c r="AJ122" s="10"/>
+      <c r="AK122" s="10"/>
+      <c r="AL122" s="10"/>
+      <c r="AM122" s="10"/>
+      <c r="AN122" s="10"/>
+      <c r="AO122" s="10"/>
+      <c r="AP122" s="10"/>
+      <c r="AQ122" s="11"/>
+    </row>
+    <row r="123" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C123" s="9"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
+      <c r="J123" s="10"/>
+      <c r="K123" s="10"/>
+      <c r="L123" s="10"/>
+      <c r="M123" s="10"/>
+      <c r="N123" s="10"/>
+      <c r="O123" s="10"/>
+      <c r="P123" s="10"/>
+      <c r="Q123" s="10"/>
+      <c r="R123" s="10"/>
+      <c r="S123" s="10"/>
+      <c r="T123" s="10"/>
+      <c r="U123" s="10"/>
+      <c r="V123" s="10"/>
+      <c r="W123" s="10"/>
+      <c r="X123" s="10"/>
+      <c r="Y123" s="10"/>
+      <c r="Z123" s="10"/>
+      <c r="AA123" s="10"/>
+      <c r="AB123" s="10"/>
+      <c r="AC123" s="10"/>
+      <c r="AD123" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE123" s="10"/>
+      <c r="AF123" s="10"/>
+      <c r="AG123" s="10"/>
+      <c r="AH123" s="10"/>
+      <c r="AI123" s="10"/>
+      <c r="AJ123" s="10"/>
+      <c r="AK123" s="10"/>
+      <c r="AL123" s="10"/>
+      <c r="AM123" s="10"/>
+      <c r="AN123" s="10"/>
+      <c r="AO123" s="10"/>
+      <c r="AP123" s="10"/>
+      <c r="AQ123" s="11"/>
+    </row>
+    <row r="124" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C124" s="9"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="10"/>
+      <c r="F124" s="10"/>
+      <c r="G124" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H124" s="10"/>
+      <c r="I124" s="10"/>
+      <c r="J124" s="10"/>
+      <c r="K124" s="10"/>
+      <c r="L124" s="10"/>
+      <c r="M124" s="10"/>
+      <c r="N124" s="10"/>
+      <c r="O124" s="10"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="10"/>
+      <c r="R124" s="10"/>
+      <c r="S124" s="10"/>
+      <c r="T124" s="10"/>
+      <c r="U124" s="10"/>
+      <c r="V124" s="10"/>
+      <c r="W124" s="10"/>
+      <c r="X124" s="10"/>
+      <c r="Y124" s="10"/>
+      <c r="Z124" s="10"/>
+      <c r="AA124" s="10"/>
+      <c r="AB124" s="10"/>
+      <c r="AC124" s="10"/>
+      <c r="AD124" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE124" s="10"/>
+      <c r="AF124" s="10"/>
+      <c r="AG124" s="10"/>
+      <c r="AH124" s="10"/>
+      <c r="AI124" s="10"/>
+      <c r="AJ124" s="10"/>
+      <c r="AK124" s="10"/>
+      <c r="AL124" s="10"/>
+      <c r="AM124" s="10"/>
+      <c r="AN124" s="10"/>
+      <c r="AO124" s="10"/>
+      <c r="AP124" s="10"/>
+      <c r="AQ124" s="11"/>
+    </row>
+    <row r="125" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C125" s="9"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="10"/>
+      <c r="F125" s="10"/>
+      <c r="G125" s="10"/>
+      <c r="H125" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I125" s="10"/>
+      <c r="J125" s="10"/>
+      <c r="K125" s="10"/>
+      <c r="L125" s="10"/>
+      <c r="M125" s="10"/>
+      <c r="N125" s="10"/>
+      <c r="O125" s="10"/>
+      <c r="P125" s="10"/>
+      <c r="Q125" s="10"/>
+      <c r="R125" s="10"/>
+      <c r="S125" s="10"/>
+      <c r="T125" s="10"/>
+      <c r="U125" s="10"/>
+      <c r="V125" s="10"/>
+      <c r="W125" s="10"/>
+      <c r="X125" s="10"/>
+      <c r="Y125" s="10"/>
+      <c r="Z125" s="10"/>
+      <c r="AA125" s="10"/>
+      <c r="AB125" s="10"/>
+      <c r="AC125" s="10"/>
+      <c r="AD125" s="10"/>
+      <c r="AE125" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF125" s="10"/>
+      <c r="AG125" s="10"/>
+      <c r="AH125" s="10"/>
+      <c r="AI125" s="10"/>
+      <c r="AJ125" s="10"/>
+      <c r="AK125" s="10"/>
+      <c r="AL125" s="10"/>
+      <c r="AM125" s="10"/>
+      <c r="AN125" s="10"/>
+      <c r="AO125" s="10"/>
+      <c r="AP125" s="10"/>
+      <c r="AQ125" s="11"/>
+    </row>
+    <row r="126" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C126" s="9"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
+      <c r="G126" s="10"/>
+      <c r="H126" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I126" s="10"/>
+      <c r="J126" s="10"/>
+      <c r="K126" s="10"/>
+      <c r="L126" s="10"/>
+      <c r="M126" s="10"/>
+      <c r="N126" s="10"/>
+      <c r="O126" s="10"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="10"/>
+      <c r="R126" s="10"/>
+      <c r="S126" s="10"/>
+      <c r="T126" s="10"/>
+      <c r="U126" s="10"/>
+      <c r="V126" s="10"/>
+      <c r="W126" s="10"/>
+      <c r="X126" s="10"/>
+      <c r="Y126" s="10"/>
+      <c r="Z126" s="10"/>
+      <c r="AA126" s="10"/>
+      <c r="AB126" s="10"/>
+      <c r="AC126" s="10"/>
+      <c r="AD126" s="10"/>
+      <c r="AE126" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF126" s="10"/>
+      <c r="AG126" s="10"/>
+      <c r="AH126" s="10"/>
+      <c r="AI126" s="10"/>
+      <c r="AJ126" s="10"/>
+      <c r="AK126" s="10"/>
+      <c r="AL126" s="10"/>
+      <c r="AM126" s="10"/>
+      <c r="AN126" s="10"/>
+      <c r="AO126" s="10"/>
+      <c r="AP126" s="10"/>
+      <c r="AQ126" s="11"/>
+    </row>
+    <row r="127" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C127" s="9"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="10"/>
+      <c r="F127" s="10"/>
+      <c r="G127" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H127" s="10"/>
+      <c r="I127" s="10"/>
+      <c r="J127" s="10"/>
+      <c r="K127" s="10"/>
+      <c r="L127" s="10"/>
+      <c r="M127" s="10"/>
+      <c r="N127" s="10"/>
+      <c r="O127" s="10"/>
+      <c r="P127" s="10"/>
+      <c r="Q127" s="10"/>
+      <c r="R127" s="10"/>
+      <c r="S127" s="10"/>
+      <c r="T127" s="10"/>
+      <c r="U127" s="10"/>
+      <c r="V127" s="10"/>
+      <c r="W127" s="10"/>
+      <c r="X127" s="10"/>
+      <c r="Y127" s="10"/>
+      <c r="Z127" s="10"/>
+      <c r="AA127" s="10"/>
+      <c r="AB127" s="10"/>
+      <c r="AC127" s="10"/>
+      <c r="AD127" s="10"/>
+      <c r="AE127" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF127" s="10"/>
+      <c r="AG127" s="10"/>
+      <c r="AH127" s="10"/>
+      <c r="AI127" s="10"/>
+      <c r="AJ127" s="10"/>
+      <c r="AK127" s="10"/>
+      <c r="AL127" s="10"/>
+      <c r="AM127" s="10"/>
+      <c r="AN127" s="10"/>
+      <c r="AO127" s="10"/>
+      <c r="AP127" s="10"/>
+      <c r="AQ127" s="11"/>
+    </row>
+    <row r="128" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C128" s="9"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H128" s="10"/>
+      <c r="I128" s="10"/>
+      <c r="J128" s="10"/>
+      <c r="K128" s="10"/>
+      <c r="L128" s="10"/>
+      <c r="M128" s="10"/>
+      <c r="N128" s="10"/>
+      <c r="O128" s="10"/>
+      <c r="P128" s="10"/>
+      <c r="Q128" s="10"/>
+      <c r="R128" s="10"/>
+      <c r="S128" s="10"/>
+      <c r="T128" s="10"/>
+      <c r="U128" s="10"/>
+      <c r="V128" s="10"/>
+      <c r="W128" s="10"/>
+      <c r="X128" s="10"/>
+      <c r="Y128" s="10"/>
+      <c r="Z128" s="10"/>
+      <c r="AA128" s="10"/>
+      <c r="AB128" s="10"/>
+      <c r="AC128" s="10"/>
+      <c r="AD128" s="10"/>
+      <c r="AE128" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF128" s="10"/>
+      <c r="AG128" s="10"/>
+      <c r="AH128" s="10"/>
+      <c r="AI128" s="10"/>
+      <c r="AJ128" s="10"/>
+      <c r="AK128" s="10"/>
+      <c r="AL128" s="10"/>
+      <c r="AM128" s="10"/>
+      <c r="AN128" s="10"/>
+      <c r="AO128" s="10"/>
+      <c r="AP128" s="10"/>
+      <c r="AQ128" s="11"/>
+    </row>
+    <row r="129" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C129" s="9"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
+      <c r="H129" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I129" s="10"/>
+      <c r="J129" s="10"/>
+      <c r="K129" s="10"/>
+      <c r="L129" s="10"/>
+      <c r="M129" s="10"/>
+      <c r="N129" s="10"/>
+      <c r="O129" s="10"/>
+      <c r="P129" s="10"/>
+      <c r="Q129" s="10"/>
+      <c r="R129" s="10"/>
+      <c r="S129" s="10"/>
+      <c r="T129" s="10"/>
+      <c r="U129" s="10"/>
+      <c r="V129" s="10"/>
+      <c r="W129" s="10"/>
+      <c r="X129" s="10"/>
+      <c r="Y129" s="10"/>
+      <c r="Z129" s="10"/>
+      <c r="AA129" s="10"/>
+      <c r="AB129" s="10"/>
+      <c r="AC129" s="10"/>
+      <c r="AD129" s="10"/>
+      <c r="AE129" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF129" s="10"/>
+      <c r="AG129" s="10"/>
+      <c r="AH129" s="10"/>
+      <c r="AI129" s="10"/>
+      <c r="AJ129" s="10"/>
+      <c r="AK129" s="10"/>
+      <c r="AL129" s="10"/>
+      <c r="AM129" s="10"/>
+      <c r="AN129" s="10"/>
+      <c r="AO129" s="10"/>
+      <c r="AP129" s="10"/>
+      <c r="AQ129" s="11"/>
+    </row>
+    <row r="130" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C130" s="9"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
+      <c r="H130" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I130" s="10"/>
+      <c r="J130" s="10"/>
+      <c r="K130" s="10"/>
+      <c r="L130" s="10"/>
+      <c r="M130" s="10"/>
+      <c r="N130" s="10"/>
+      <c r="O130" s="10"/>
+      <c r="P130" s="10"/>
+      <c r="Q130" s="10"/>
+      <c r="R130" s="10"/>
+      <c r="S130" s="10"/>
+      <c r="T130" s="10"/>
+      <c r="U130" s="10"/>
+      <c r="V130" s="10"/>
+      <c r="W130" s="10"/>
+      <c r="X130" s="10"/>
+      <c r="Y130" s="10"/>
+      <c r="Z130" s="10"/>
+      <c r="AA130" s="10"/>
+      <c r="AB130" s="10"/>
+      <c r="AC130" s="10"/>
+      <c r="AD130" s="10"/>
+      <c r="AE130" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF130" s="10"/>
+      <c r="AG130" s="10"/>
+      <c r="AH130" s="10"/>
+      <c r="AI130" s="10"/>
+      <c r="AJ130" s="10"/>
+      <c r="AK130" s="10"/>
+      <c r="AL130" s="10"/>
+      <c r="AM130" s="10"/>
+      <c r="AN130" s="10"/>
+      <c r="AO130" s="10"/>
+      <c r="AP130" s="10"/>
+      <c r="AQ130" s="11"/>
+    </row>
+    <row r="131" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C131" s="9"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H131" s="10"/>
+      <c r="I131" s="10"/>
+      <c r="J131" s="10"/>
+      <c r="K131" s="10"/>
+      <c r="L131" s="10"/>
+      <c r="M131" s="10"/>
+      <c r="N131" s="10"/>
+      <c r="O131" s="10"/>
+      <c r="P131" s="10"/>
+      <c r="Q131" s="10"/>
+      <c r="R131" s="10"/>
+      <c r="S131" s="10"/>
+      <c r="T131" s="10"/>
+      <c r="U131" s="10"/>
+      <c r="V131" s="10"/>
+      <c r="W131" s="10"/>
+      <c r="X131" s="10"/>
+      <c r="Y131" s="10"/>
+      <c r="Z131" s="10"/>
+      <c r="AA131" s="10"/>
+      <c r="AB131" s="10"/>
+      <c r="AC131" s="10"/>
+      <c r="AD131" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE131" s="10"/>
+      <c r="AF131" s="10"/>
+      <c r="AG131" s="10"/>
+      <c r="AH131" s="10"/>
+      <c r="AI131" s="10"/>
+      <c r="AJ131" s="10"/>
+      <c r="AK131" s="10"/>
+      <c r="AL131" s="10"/>
+      <c r="AM131" s="10"/>
+      <c r="AN131" s="10"/>
+      <c r="AO131" s="10"/>
+      <c r="AP131" s="10"/>
+      <c r="AQ131" s="11"/>
+    </row>
+    <row r="132" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C132" s="9"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H132" s="10"/>
+      <c r="I132" s="10"/>
+      <c r="J132" s="10"/>
+      <c r="K132" s="10"/>
+      <c r="L132" s="10"/>
+      <c r="M132" s="10"/>
+      <c r="N132" s="10"/>
+      <c r="O132" s="10"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="10"/>
+      <c r="R132" s="10"/>
+      <c r="S132" s="10"/>
+      <c r="T132" s="10"/>
+      <c r="U132" s="10"/>
+      <c r="V132" s="10"/>
+      <c r="W132" s="10"/>
+      <c r="X132" s="10"/>
+      <c r="Y132" s="10"/>
+      <c r="Z132" s="10"/>
+      <c r="AA132" s="10"/>
+      <c r="AB132" s="10"/>
+      <c r="AC132" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD132" s="10"/>
+      <c r="AE132" s="10"/>
+      <c r="AF132" s="10"/>
+      <c r="AG132" s="10"/>
+      <c r="AH132" s="10"/>
+      <c r="AI132" s="10"/>
+      <c r="AJ132" s="10"/>
+      <c r="AK132" s="10"/>
+      <c r="AL132" s="10"/>
+      <c r="AM132" s="10"/>
+      <c r="AN132" s="10"/>
+      <c r="AO132" s="10"/>
+      <c r="AP132" s="10"/>
+      <c r="AQ132" s="11"/>
+    </row>
+    <row r="133" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C133" s="9"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
+      <c r="J133" s="10"/>
+      <c r="K133" s="10"/>
+      <c r="L133" s="10"/>
+      <c r="M133" s="10"/>
+      <c r="N133" s="10"/>
+      <c r="O133" s="10"/>
+      <c r="P133" s="10"/>
+      <c r="Q133" s="10"/>
+      <c r="R133" s="10"/>
+      <c r="S133" s="10"/>
+      <c r="T133" s="10"/>
+      <c r="U133" s="10"/>
+      <c r="V133" s="10"/>
+      <c r="W133" s="10"/>
+      <c r="X133" s="10"/>
+      <c r="Y133" s="10"/>
+      <c r="Z133" s="10"/>
+      <c r="AA133" s="10"/>
+      <c r="AB133" s="10"/>
+      <c r="AC133" s="10"/>
+      <c r="AD133" s="10"/>
+      <c r="AE133" s="10"/>
+      <c r="AF133" s="10"/>
+      <c r="AG133" s="10"/>
+      <c r="AH133" s="10"/>
+      <c r="AI133" s="10"/>
+      <c r="AJ133" s="10"/>
+      <c r="AK133" s="10"/>
+      <c r="AL133" s="10"/>
+      <c r="AM133" s="10"/>
+      <c r="AN133" s="10"/>
+      <c r="AO133" s="10"/>
+      <c r="AP133" s="10"/>
+      <c r="AQ133" s="11"/>
+    </row>
+    <row r="134" spans="3:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C134" s="12"/>
+      <c r="D134" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="13"/>
+      <c r="K134" s="13"/>
+      <c r="L134" s="13"/>
+      <c r="M134" s="13"/>
+      <c r="N134" s="13"/>
+      <c r="O134" s="13"/>
+      <c r="P134" s="13"/>
+      <c r="Q134" s="13"/>
+      <c r="R134" s="13"/>
+      <c r="S134" s="13"/>
+      <c r="T134" s="13"/>
+      <c r="U134" s="13"/>
+      <c r="V134" s="13"/>
+      <c r="W134" s="13"/>
+      <c r="X134" s="13"/>
+      <c r="Y134" s="13"/>
+      <c r="Z134" s="13"/>
+      <c r="AA134" s="13"/>
+      <c r="AB134" s="13"/>
+      <c r="AC134" s="13"/>
+      <c r="AD134" s="13"/>
+      <c r="AE134" s="13"/>
+      <c r="AF134" s="13"/>
+      <c r="AG134" s="13"/>
+      <c r="AH134" s="13"/>
+      <c r="AI134" s="13"/>
+      <c r="AJ134" s="13"/>
+      <c r="AK134" s="13"/>
+      <c r="AL134" s="13"/>
+      <c r="AM134" s="13"/>
+      <c r="AN134" s="13"/>
+      <c r="AO134" s="13"/>
+      <c r="AP134" s="13"/>
+      <c r="AQ134" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -6691,8 +8896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6702,17 +8907,17 @@
   <sheetData>
     <row r="2" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C3" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -6722,42 +8927,42 @@
     </row>
     <row r="7" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D7" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="T7" s="15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E8" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="T8" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E9" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="T9" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E10" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="T10" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E11" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="T11" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -6767,90 +8972,90 @@
     </row>
     <row r="13" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D13" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T13" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E14" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="T14" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E15" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T15" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E16" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="T16" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E17" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="T17" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F18" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T18" s="15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F19" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T19" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F20" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="T20" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F21" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="T21" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F22" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T22" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F23" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="T23" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -6860,124 +9065,124 @@
     </row>
     <row r="25" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D25" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E26" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="T26" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E27" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="T27" s="15" t="s">
         <v>196</v>
-      </c>
-      <c r="T27" s="15" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="28" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E28" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="T28" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="T28" s="15" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="29" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D29" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D30" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="T30" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E31" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="T31" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="T31" s="15" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="32" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D32" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D33" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="T33" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E34" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T34" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E35" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="T35" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E36" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T36" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E37" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="T37" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E38" s="15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T38" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E39" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="T39" s="15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E40" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T40" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -6987,82 +9192,82 @@
     </row>
     <row r="42" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D42" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="T42" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E43" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T43" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E44" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T44" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E45" s="15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="T45" s="15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E46" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T46" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="47" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E47" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="T47" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="4:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E48" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T48" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E49" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="T49" s="15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E50" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T50" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E51" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="T51" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -7072,68 +9277,68 @@
     </row>
     <row r="53" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D53" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="T53" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="54" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E54" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="T54" s="15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F55" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="T55" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="56" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F56" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="T56" s="15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F57" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="T57" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E58" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E59" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T59" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F60" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="T60" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="T60" s="15" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="61" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E61" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="3:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -7148,93 +9353,93 @@
     </row>
     <row r="65" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C66" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D67" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="T67" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D68" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="T68" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D69" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="T69" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D70" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T70" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="71" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D71" s="15" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="T71" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="72" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E72" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E73" s="15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D74" s="15" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="T74" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="75" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E75" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E76" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="77" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D77" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="T77" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="E78" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
base environment for AI Model SDK
</commit_message>
<xml_diff>
--- a/figure/figure.xlsx
+++ b/figure/figure.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25965" windowHeight="10320" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20760" windowHeight="11790" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="2" r:id="rId1"/>
     <sheet name="django_admin_before_after" sheetId="1" r:id="rId2"/>
     <sheet name="custom_dataset_format" sheetId="3" r:id="rId3"/>
     <sheet name="config_file_structure" sheetId="4" r:id="rId4"/>
+    <sheet name="ai_model_sdk_specification" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="239">
   <si>
     <t>Before</t>
     <phoneticPr fontId="1"/>
@@ -872,6 +873,82 @@
   </si>
   <si>
     <t>"dtype": &lt;"int", "float", "str", "list"&gt;,</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AI Model SDK Specifications Overview</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class AI_Model_SDK()</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def __init__():</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constructor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Preprocessing data sample</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def  preprocess_data(data_sample):</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def load_dataset(dataset):</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def build_model():</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def train_model():</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def eval_model():</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Evaluate model</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Train model</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If nessesary, set pre-trained parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Build model and training strategy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Load and preprocess dataset for training or evaluation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>- Initialize parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>- Define the configurable parameters and create config file using on Web UI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>def predict():</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Predict each data sample</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -879,7 +956,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -925,6 +1002,22 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="メイリオ"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
@@ -1035,7 +1128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1077,12 +1170,20 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3333FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3862,6 +3963,1523 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>235322</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>235323</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1647265" y="470646"/>
+          <a:ext cx="8471647" cy="3529853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>AI Dashboard</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>235321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>235322</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="8" name="グループ化 7"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1882588" y="1176615"/>
+          <a:ext cx="2823883" cy="2823883"/>
+          <a:chOff x="952501" y="952498"/>
+          <a:chExt cx="2857500" cy="2857503"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="952501" y="952498"/>
+            <a:ext cx="2857500" cy="2857503"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:rPr>
+              <a:t>app</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="7" name="グループ化 6"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1190625" y="1428750"/>
+            <a:ext cx="2381250" cy="2143127"/>
+            <a:chOff x="1666876" y="1428750"/>
+            <a:chExt cx="2381250" cy="2143127"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1666876" y="1428750"/>
+              <a:ext cx="2381250" cy="2143127"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:rPr>
+                <a:t>machine_learning</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1905000" y="1905001"/>
+              <a:ext cx="952500" cy="238124"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:rPr>
+                <a:t>main.py</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="正方形/長方形 5"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3095625" y="1905001"/>
+              <a:ext cx="714376" cy="238124"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:rPr>
+                <a:t>lib</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="正方形/長方形 18"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1904999" y="2381251"/>
+              <a:ext cx="1905001" cy="952499"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr"/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+                  <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                  <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                </a:rPr>
+                <a:t>(Web UI)</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+                <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+                <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>235322</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>235322</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3765176" y="941293"/>
+          <a:ext cx="4941796" cy="2353235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>media</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="1411941"/>
+          <a:ext cx="1647265" cy="1647266"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>ai_model_sdk</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5883089" y="1411941"/>
+          <a:ext cx="1176618" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>config</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5883088" y="2117912"/>
+          <a:ext cx="1176618" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>dataset</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>235322</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7295029" y="1411941"/>
+          <a:ext cx="1176617" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>model</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>235322</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7295029" y="2117912"/>
+          <a:ext cx="1176617" cy="470647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>notebooks</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>235323</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="正方形/長方形 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="1882588"/>
+          <a:ext cx="1176618" cy="235323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>ModelA SDK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>235323</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="正方形/長方形 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="2353235"/>
+          <a:ext cx="1176618" cy="235323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>ModelB SDK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>117662</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>93720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>117662</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>130391</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="直線コネクタ 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4824133" y="2682279"/>
+          <a:ext cx="0" cy="271994"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDot"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>24620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171130</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>145467</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="図 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="259944" y="2524365"/>
+          <a:ext cx="1062141" cy="808827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>235322</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="直線コネクタ 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2823881" y="2117912"/>
+          <a:ext cx="1" cy="235323"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>112059</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="直線コネクタ 24"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3877234" y="2117912"/>
+          <a:ext cx="1" cy="235323"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>160925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>48866</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="フローチャート: 判断 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2454088" y="2749484"/>
+          <a:ext cx="1075765" cy="358588"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>SDK Selector</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>145467</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104897</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="直線コネクタ 27"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="20" idx="1"/>
+          <a:endCxn id="26" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1322085" y="2928778"/>
+          <a:ext cx="1132003" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="3333FF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11206</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>11205</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1797993" cy="325217"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="テキスト ボックス 28"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1187824" y="2599764"/>
+          <a:ext cx="1797993" cy="325217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="127000">
+                  <a:schemeClr val="bg1"/>
+                </a:glow>
+              </a:effectLst>
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Choose AI Model SDK</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:glow rad="127000">
+                <a:schemeClr val="bg1"/>
+              </a:glow>
+            </a:effectLst>
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168090</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>117663</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>48866</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="カギ線コネクタ 31"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="2"/>
+          <a:endCxn id="26" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="4471929" y="1579250"/>
+          <a:ext cx="48865" cy="3008779"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 705413"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="3333FF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168089</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168089</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>160925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="直線矢印コネクタ 34"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="26" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2991971" y="2117912"/>
+          <a:ext cx="0" cy="631572"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="3333FF"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>212913</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>145675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2825004" cy="325217"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="テキスト ボックス 35"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="212913" y="2263587"/>
+          <a:ext cx="2825004" cy="325217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="3333FF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:glow rad="127000">
+                  <a:schemeClr val="bg1"/>
+                </a:glow>
+              </a:effectLst>
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Set Model SDK Path to Python Path</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="3333FF"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:glow rad="127000">
+                <a:schemeClr val="bg1"/>
+              </a:glow>
+            </a:effectLst>
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>33617</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179296</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="四角形吹き出し 36"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5121088" y="403413"/>
+          <a:ext cx="3619500" cy="481854"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -26793"/>
+            <a:gd name="adj2" fmla="val 83135"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="3333FF"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>Training Model with Choosed AI Model SDK</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            </a:rPr>
+            <a:t>and Save to "model" directory</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="50" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>228973</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>124011</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="カギ線コネクタ 37"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="0"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipV="1">
+          <a:off x="6177242" y="-1470772"/>
+          <a:ext cx="12700" cy="5765426"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 4447055"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="3333FF"/>
+          </a:solidFill>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
@@ -4199,7 +5817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AQ134"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="AY85" sqref="AY85"/>
     </sheetView>
   </sheetViews>
@@ -8904,7 +10522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -9468,4 +11086,120 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F21:J45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM33" sqref="AM33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="3.125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="21" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="17" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J26" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H28" s="17" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="17" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="17" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="41" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="17" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>